<commit_message>
Update Ultimate Excel Gantt Chart 7 days.xlsx
Bugfix on 7 days  Gantt chart stages selection list.
</commit_message>
<xml_diff>
--- a/Ultimate Excel Gantt Chart 7 days.xlsx
+++ b/Ultimate Excel Gantt Chart 7 days.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Repos\UltiExcelGantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704EF840-AA18-4977-A2A3-0A2C516D96DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BBBB70-BBB2-436F-A2A1-00A436A47929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{FFDBE86C-E0AC-4E7A-ABF5-EFB3D0056DD5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{FFDBE86C-E0AC-4E7A-ABF5-EFB3D0056DD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="137">
   <si>
     <t>ids</t>
   </si>
@@ -447,9 +447,6 @@
     <t>Non working day (Filtered)</t>
   </si>
   <si>
-    <t>Work Order</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -460,9 +457,6 @@
   </si>
   <si>
     <t>Filter 5</t>
-  </si>
-  <si>
-    <t>WO</t>
   </si>
   <si>
     <t>Holiday 1</t>
@@ -489,34 +483,7 @@
     <t>Filter 8</t>
   </si>
   <si>
-    <t>Rollout prep</t>
-  </si>
-  <si>
     <t>Filtered</t>
-  </si>
-  <si>
-    <t>Release</t>
-  </si>
-  <si>
-    <t>1032  TTV  AOI #1</t>
-  </si>
-  <si>
-    <t>1033  TTV  AOI #2</t>
-  </si>
-  <si>
-    <t>1032  TTV  AOI #3</t>
-  </si>
-  <si>
-    <t>1033  TTV  AOI #4</t>
-  </si>
-  <si>
-    <t>1034  TTV  AOI #5</t>
-  </si>
-  <si>
-    <t>1035  TTV  AOI #6</t>
-  </si>
-  <si>
-    <t>1036  TTV  AOI #7</t>
   </si>
   <si>
     <t>I spent 4 hours of my weekend time to create this Gantt chart by following Youtube link below.</t>
@@ -559,6 +526,15 @@
   </si>
   <si>
     <t>edward-0116/UltiExcelGantt: Ultimate Excel Gantt Chart (github.com)</t>
+  </si>
+  <si>
+    <t>Stages</t>
+  </si>
+  <si>
+    <t>Rollout prep</t>
+  </si>
+  <si>
+    <t>Release</t>
   </si>
 </sst>
 </file>
@@ -1364,6 +1340,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color theme="0" tint="-0.24994659260841701"/>
       </left>
@@ -1387,24 +1381,6 @@
       <bottom style="thin">
         <color theme="0"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1633,16 +1609,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="7" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1655,12 +1622,12 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="15" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="15" fillId="4" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="15" fillId="4" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="22" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="15" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="15" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="15" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1673,6 +1640,15 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1687,42 +1663,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1746,6 +1686,42 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="21" fillId="16" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1850,84 +1826,44 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="\◆"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF1B6D4A"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF28A470"/>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF1B6D4A"/>
+        <color rgb="FF0A3F87"/>
       </font>
       <numFmt numFmtId="167" formatCode="\◆"/>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF89860C"/>
+          <bgColor rgb="FF0E5FCB"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFCDC912"/>
+          <bgColor rgb="FF0A3F87"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF89860C"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="\◆"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF845C02"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC58A03"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF845C02"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="\◆"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF840441"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC60662"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF840441"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="\◆"/>
     </dxf>
     <dxf>
       <font>
@@ -1950,42 +1886,82 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF840441"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="\◆"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF0A3F87"/>
+          <bgColor rgb="FFC60662"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF0E5FCB"/>
+          <bgColor rgb="FF840441"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF0A3F87"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="\◆"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color rgb="FF845C02"/>
       </font>
       <numFmt numFmtId="167" formatCode="\◆"/>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
+          <bgColor rgb="FFC58A03"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
+          <bgColor rgb="FF845C02"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF89860C"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="\◆"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCDC912"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF89860C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF1B6D4A"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="\◆"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF28A470"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF1B6D4A"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2215,6 +2191,90 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF0E5FCB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0A3F87"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6C288A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF481B5C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC60662"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF840441"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC58A03"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF845C02"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCDC912"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF89860C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF28A470"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF1B6D4A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFF3F082"/>
         </patternFill>
       </fill>
@@ -2332,90 +2392,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF28A470"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF1B6D4A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCDC912"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF89860C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC58A03"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF845C02"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC60662"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF840441"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6C288A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF481B5C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0E5FCB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0A3F87"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="168" formatCode="\ \ \ @"/>
     </dxf>
     <dxf>
@@ -2485,7 +2461,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>959926</xdr:colOff>
+      <xdr:colOff>973261</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>34920</xdr:rowOff>
     </xdr:to>
@@ -2996,7 +2972,7 @@
   <dimension ref="B1:AI203"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD35"/>
+      <selection activeCell="AG1" sqref="AG1:AI1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3091,7 +3067,7 @@
       <c r="AD6" s="133"/>
       <c r="AE6" s="133"/>
       <c r="AG6" s="133" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="AH6" s="133"/>
       <c r="AI6" s="133"/>
@@ -3160,28 +3136,28 @@
         <v>7</v>
       </c>
       <c r="U8" s="102" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="V8" s="8"/>
       <c r="X8" s="98"/>
       <c r="Y8" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Z8" s="103" t="s">
         <v>66</v>
       </c>
       <c r="AA8" s="104" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB8" s="9" t="s">
         <v>110</v>
-      </c>
-      <c r="AB8" s="9" t="s">
-        <v>111</v>
       </c>
       <c r="AC8" s="103"/>
       <c r="AD8" s="104"/>
       <c r="AE8" s="100"/>
       <c r="AG8" s="6"/>
-      <c r="AH8" s="105" t="s">
-        <v>112</v>
+      <c r="AH8" s="130" t="s">
+        <v>134</v>
       </c>
       <c r="AI8" s="8"/>
     </row>
@@ -3216,30 +3192,30 @@
       <c r="Q9" s="8"/>
       <c r="S9" s="6"/>
       <c r="T9" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="U9" s="106">
+        <v>111</v>
+      </c>
+      <c r="U9" s="105">
         <v>44489</v>
       </c>
       <c r="V9" s="8"/>
       <c r="X9" s="98"/>
       <c r="Y9" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="Z9" s="103" t="s">
         <v>67</v>
       </c>
       <c r="AA9" s="104" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AB9" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AC9" s="103"/>
       <c r="AD9" s="104"/>
       <c r="AE9" s="100"/>
       <c r="AG9" s="6"/>
-      <c r="AH9" s="107" t="s">
+      <c r="AH9" s="131" t="s">
         <v>94</v>
       </c>
       <c r="AI9" s="8"/>
@@ -3279,30 +3255,30 @@
       <c r="Q10" s="8"/>
       <c r="S10" s="6"/>
       <c r="T10" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="U10" s="106">
+        <v>114</v>
+      </c>
+      <c r="U10" s="105">
         <v>44504</v>
       </c>
       <c r="V10" s="8"/>
       <c r="X10" s="6"/>
       <c r="Y10" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="Z10" s="103" t="s">
         <v>69</v>
       </c>
       <c r="AA10" s="104" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AB10" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AC10" s="103"/>
       <c r="AD10" s="104"/>
       <c r="AE10" s="8"/>
       <c r="AG10" s="6"/>
-      <c r="AH10" s="108" t="s">
+      <c r="AH10" s="132" t="s">
         <v>46</v>
       </c>
       <c r="AI10" s="8"/>
@@ -3338,23 +3314,23 @@
       <c r="Q11" s="8"/>
       <c r="S11" s="6"/>
       <c r="T11" s="58"/>
-      <c r="U11" s="106"/>
+      <c r="U11" s="105"/>
       <c r="V11" s="8"/>
       <c r="X11" s="98"/>
       <c r="Y11" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Z11" s="103"/>
       <c r="AA11" s="104"/>
       <c r="AB11" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AC11" s="103"/>
       <c r="AD11" s="104"/>
       <c r="AE11" s="100"/>
       <c r="AG11" s="6"/>
-      <c r="AH11" s="108" t="s">
-        <v>121</v>
+      <c r="AH11" s="132" t="s">
+        <v>135</v>
       </c>
       <c r="AI11" s="8"/>
     </row>
@@ -3393,12 +3369,12 @@
       <c r="Q12" s="8"/>
       <c r="S12" s="6"/>
       <c r="T12" s="58"/>
-      <c r="U12" s="106"/>
+      <c r="U12" s="105"/>
       <c r="V12" s="8"/>
       <c r="X12" s="6"/>
       <c r="AE12" s="8"/>
       <c r="AG12" s="6"/>
-      <c r="AH12" s="108" t="s">
+      <c r="AH12" s="132" t="s">
         <v>81</v>
       </c>
       <c r="AI12" s="8"/>
@@ -3434,26 +3410,26 @@
       <c r="Q13" s="8"/>
       <c r="S13" s="6"/>
       <c r="T13" s="58"/>
-      <c r="U13" s="106"/>
+      <c r="U13" s="105"/>
       <c r="V13" s="8"/>
       <c r="X13" s="6"/>
       <c r="Y13" s="101" t="s">
         <v>7</v>
       </c>
       <c r="Z13" s="101" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA13" s="109" t="s">
-        <v>122</v>
-      </c>
-      <c r="AB13" s="110" t="s">
-        <v>122</v>
-      </c>
-      <c r="AC13" s="111"/>
-      <c r="AD13" s="112"/>
+        <v>107</v>
+      </c>
+      <c r="AA13" s="106" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB13" s="107" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC13" s="108"/>
+      <c r="AD13" s="109"/>
       <c r="AE13" s="8"/>
       <c r="AG13" s="6"/>
-      <c r="AH13" s="108" t="s">
+      <c r="AH13" s="132" t="s">
         <v>95</v>
       </c>
       <c r="AI13" s="8"/>
@@ -3485,29 +3461,29 @@
       <c r="Q14" s="8"/>
       <c r="S14" s="6"/>
       <c r="T14" s="58"/>
-      <c r="U14" s="106"/>
+      <c r="U14" s="105"/>
       <c r="V14" s="8"/>
       <c r="X14" s="6"/>
-      <c r="Y14" s="113" t="s">
+      <c r="Y14" s="110" t="s">
         <v>66</v>
       </c>
-      <c r="Z14" s="114">
+      <c r="Z14" s="111">
         <v>44524</v>
       </c>
-      <c r="AA14" s="115">
+      <c r="AA14" s="112">
         <f t="shared" ref="AA14:AA58" si="2">IF(OR(AND($AA$8="✔",Y14=$Z$8),AND($AA$9="✔",Y14=$Z$9),AND($AA$10="✔",Y14=$Z$10),AND($AA$11="✔",Y14=$Z$11),AND($AD$8="✔",Y14=$AC$8),AND($AD$9="✔",Y14=$AC$9),AND($AD$10="✔",Y14=$AC$10),AND($AD$11="✔",Y14=$AC$11)),Z14,"")</f>
         <v>44524</v>
       </c>
-      <c r="AB14" s="116" cm="1">
+      <c r="AB14" s="113" cm="1">
         <f t="array" ref="AB14:AB16">_xlfn._xlws.FILTER(Z14:Z59,((Y14:Y59=$Z$8)*(Y14:Y59&lt;&gt;""))+((Y14:Y59=$Z$9)*(Y14:Y59&lt;&gt;""))+((Y14:Y59=$Z$10)*(Y14:Y59&lt;&gt;""))+((Y14:Y59=$Z$11)*(Y14:Y59&lt;&gt;""))+((Y14:Y59=$AC$8)*(Y14:Y59&lt;&gt;""))+((Y14:Y59=$AC$9)*(Y14:Y59&lt;&gt;""))+((Y14:Y59=$AC$10)*(Y14:Y59&lt;&gt;""))+((Y14:Y59=$AC$11)*(Y14:Y59&lt;&gt;"")),"")</f>
         <v>44524</v>
       </c>
-      <c r="AC14" s="111"/>
-      <c r="AD14" s="117"/>
+      <c r="AC14" s="108"/>
+      <c r="AD14" s="114"/>
       <c r="AE14" s="8"/>
       <c r="AG14" s="6"/>
-      <c r="AH14" s="108" t="s">
-        <v>123</v>
+      <c r="AH14" s="132" t="s">
+        <v>136</v>
       </c>
       <c r="AI14" s="8"/>
     </row>
@@ -3534,29 +3510,27 @@
       <c r="Q15" s="8"/>
       <c r="S15" s="6"/>
       <c r="T15" s="58"/>
-      <c r="U15" s="106"/>
+      <c r="U15" s="105"/>
       <c r="V15" s="8"/>
       <c r="X15" s="6"/>
-      <c r="Y15" s="113" t="s">
+      <c r="Y15" s="110" t="s">
         <v>67</v>
       </c>
-      <c r="Z15" s="114">
+      <c r="Z15" s="111">
         <v>44512</v>
       </c>
-      <c r="AA15" s="118">
+      <c r="AA15" s="115">
         <f t="shared" si="2"/>
         <v>44512</v>
       </c>
-      <c r="AB15" s="116">
+      <c r="AB15" s="113">
         <v>44512</v>
       </c>
-      <c r="AC15" s="111"/>
-      <c r="AD15" s="117"/>
+      <c r="AC15" s="108"/>
+      <c r="AD15" s="114"/>
       <c r="AE15" s="8"/>
       <c r="AG15" s="6"/>
-      <c r="AH15" s="108" t="s">
-        <v>124</v>
-      </c>
+      <c r="AH15" s="132"/>
       <c r="AI15" s="8"/>
     </row>
     <row r="16" spans="2:35" x14ac:dyDescent="0.3">
@@ -3578,29 +3552,27 @@
       <c r="Q16" s="8"/>
       <c r="S16" s="6"/>
       <c r="T16" s="58"/>
-      <c r="U16" s="106"/>
+      <c r="U16" s="105"/>
       <c r="V16" s="8"/>
       <c r="X16" s="6"/>
-      <c r="Y16" s="113" t="s">
+      <c r="Y16" s="110" t="s">
         <v>69</v>
       </c>
-      <c r="Z16" s="114">
+      <c r="Z16" s="111">
         <v>44496</v>
       </c>
-      <c r="AA16" s="118">
+      <c r="AA16" s="115">
         <f t="shared" si="2"/>
         <v>44496</v>
       </c>
-      <c r="AB16" s="116">
+      <c r="AB16" s="113">
         <v>44496</v>
       </c>
-      <c r="AC16" s="111"/>
-      <c r="AD16" s="117"/>
+      <c r="AC16" s="108"/>
+      <c r="AD16" s="114"/>
       <c r="AE16" s="8"/>
       <c r="AG16" s="6"/>
-      <c r="AH16" s="108" t="s">
-        <v>125</v>
-      </c>
+      <c r="AH16" s="132"/>
       <c r="AI16" s="8"/>
     </row>
     <row r="17" spans="2:35" x14ac:dyDescent="0.3">
@@ -3622,23 +3594,21 @@
       <c r="Q17" s="8"/>
       <c r="S17" s="6"/>
       <c r="T17" s="58"/>
-      <c r="U17" s="106"/>
+      <c r="U17" s="105"/>
       <c r="V17" s="8"/>
       <c r="X17" s="6"/>
-      <c r="Y17" s="113"/>
-      <c r="Z17" s="114"/>
-      <c r="AA17" s="118" t="str">
+      <c r="Y17" s="110"/>
+      <c r="Z17" s="111"/>
+      <c r="AA17" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB17" s="116"/>
-      <c r="AC17" s="111"/>
-      <c r="AD17" s="117"/>
+      <c r="AB17" s="113"/>
+      <c r="AC17" s="108"/>
+      <c r="AD17" s="114"/>
       <c r="AE17" s="8"/>
       <c r="AG17" s="6"/>
-      <c r="AH17" s="108" t="s">
-        <v>126</v>
-      </c>
+      <c r="AH17" s="132"/>
       <c r="AI17" s="8"/>
     </row>
     <row r="18" spans="2:35" x14ac:dyDescent="0.3">
@@ -3660,23 +3630,21 @@
       <c r="Q18" s="8"/>
       <c r="S18" s="6"/>
       <c r="T18" s="58"/>
-      <c r="U18" s="106"/>
+      <c r="U18" s="105"/>
       <c r="V18" s="8"/>
       <c r="X18" s="6"/>
-      <c r="Y18" s="113"/>
-      <c r="Z18" s="114"/>
-      <c r="AA18" s="118" t="str">
+      <c r="Y18" s="110"/>
+      <c r="Z18" s="111"/>
+      <c r="AA18" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB18" s="116"/>
-      <c r="AC18" s="111"/>
-      <c r="AD18" s="117"/>
+      <c r="AB18" s="113"/>
+      <c r="AC18" s="108"/>
+      <c r="AD18" s="114"/>
       <c r="AE18" s="8"/>
       <c r="AG18" s="6"/>
-      <c r="AH18" s="108" t="s">
-        <v>127</v>
-      </c>
+      <c r="AH18" s="132"/>
       <c r="AI18" s="8"/>
     </row>
     <row r="19" spans="2:35" x14ac:dyDescent="0.3">
@@ -3698,23 +3666,21 @@
       <c r="Q19" s="8"/>
       <c r="S19" s="6"/>
       <c r="T19" s="58"/>
-      <c r="U19" s="106"/>
+      <c r="U19" s="105"/>
       <c r="V19" s="8"/>
       <c r="X19" s="6"/>
-      <c r="Y19" s="113"/>
-      <c r="Z19" s="114"/>
-      <c r="AA19" s="118" t="str">
+      <c r="Y19" s="110"/>
+      <c r="Z19" s="111"/>
+      <c r="AA19" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB19" s="116"/>
-      <c r="AC19" s="111"/>
-      <c r="AD19" s="117"/>
+      <c r="AB19" s="113"/>
+      <c r="AC19" s="108"/>
+      <c r="AD19" s="114"/>
       <c r="AE19" s="8"/>
       <c r="AG19" s="6"/>
-      <c r="AH19" s="108" t="s">
-        <v>128</v>
-      </c>
+      <c r="AH19" s="132"/>
       <c r="AI19" s="8"/>
     </row>
     <row r="20" spans="2:35" x14ac:dyDescent="0.3">
@@ -3736,23 +3702,21 @@
       <c r="Q20" s="8"/>
       <c r="S20" s="6"/>
       <c r="T20" s="58"/>
-      <c r="U20" s="106"/>
+      <c r="U20" s="105"/>
       <c r="V20" s="8"/>
       <c r="X20" s="6"/>
-      <c r="Y20" s="113"/>
-      <c r="Z20" s="114"/>
-      <c r="AA20" s="118" t="str">
+      <c r="Y20" s="110"/>
+      <c r="Z20" s="111"/>
+      <c r="AA20" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB20" s="116"/>
-      <c r="AC20" s="111"/>
-      <c r="AD20" s="117"/>
+      <c r="AB20" s="113"/>
+      <c r="AC20" s="108"/>
+      <c r="AD20" s="114"/>
       <c r="AE20" s="8"/>
       <c r="AG20" s="6"/>
-      <c r="AH20" s="108" t="s">
-        <v>129</v>
-      </c>
+      <c r="AH20" s="132"/>
       <c r="AI20" s="8"/>
     </row>
     <row r="21" spans="2:35" x14ac:dyDescent="0.3">
@@ -3774,23 +3738,21 @@
       <c r="Q21" s="8"/>
       <c r="S21" s="6"/>
       <c r="T21" s="58"/>
-      <c r="U21" s="106"/>
+      <c r="U21" s="105"/>
       <c r="V21" s="8"/>
       <c r="X21" s="6"/>
-      <c r="Y21" s="113"/>
-      <c r="Z21" s="114"/>
-      <c r="AA21" s="118" t="str">
+      <c r="Y21" s="110"/>
+      <c r="Z21" s="111"/>
+      <c r="AA21" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB21" s="116"/>
-      <c r="AC21" s="111"/>
-      <c r="AD21" s="117"/>
+      <c r="AB21" s="113"/>
+      <c r="AC21" s="108"/>
+      <c r="AD21" s="114"/>
       <c r="AE21" s="8"/>
       <c r="AG21" s="6"/>
-      <c r="AH21" s="108" t="s">
-        <v>130</v>
-      </c>
+      <c r="AH21" s="132"/>
       <c r="AI21" s="8"/>
     </row>
     <row r="22" spans="2:35" x14ac:dyDescent="0.3">
@@ -3812,23 +3774,21 @@
       <c r="Q22" s="8"/>
       <c r="S22" s="6"/>
       <c r="T22" s="58"/>
-      <c r="U22" s="106"/>
+      <c r="U22" s="105"/>
       <c r="V22" s="8"/>
       <c r="X22" s="6"/>
-      <c r="Y22" s="113"/>
-      <c r="Z22" s="114"/>
-      <c r="AA22" s="118" t="str">
+      <c r="Y22" s="110"/>
+      <c r="Z22" s="111"/>
+      <c r="AA22" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB22" s="116"/>
-      <c r="AC22" s="111"/>
-      <c r="AD22" s="117"/>
+      <c r="AB22" s="113"/>
+      <c r="AC22" s="108"/>
+      <c r="AD22" s="114"/>
       <c r="AE22" s="8"/>
       <c r="AG22" s="6"/>
-      <c r="AH22" s="108" t="s">
-        <v>128</v>
-      </c>
+      <c r="AH22" s="132"/>
       <c r="AI22" s="8"/>
     </row>
     <row r="23" spans="2:35" x14ac:dyDescent="0.3">
@@ -3847,29 +3807,27 @@
       <c r="Q23" s="8"/>
       <c r="S23" s="6"/>
       <c r="T23" s="58"/>
-      <c r="U23" s="106"/>
+      <c r="U23" s="105"/>
       <c r="V23" s="8"/>
       <c r="X23" s="6"/>
-      <c r="Y23" s="113"/>
-      <c r="Z23" s="114"/>
-      <c r="AA23" s="118" t="str">
+      <c r="Y23" s="110"/>
+      <c r="Z23" s="111"/>
+      <c r="AA23" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB23" s="116"/>
-      <c r="AC23" s="111"/>
-      <c r="AD23" s="117"/>
+      <c r="AB23" s="113"/>
+      <c r="AC23" s="108"/>
+      <c r="AD23" s="114"/>
       <c r="AE23" s="8"/>
       <c r="AG23" s="6"/>
-      <c r="AH23" s="108" t="s">
-        <v>129</v>
-      </c>
+      <c r="AH23" s="132"/>
       <c r="AI23" s="8"/>
     </row>
     <row r="24" spans="2:35" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B24" s="123"/>
-      <c r="G24" s="129" t="s">
-        <v>142</v>
+      <c r="B24" s="120"/>
+      <c r="G24" s="126" t="s">
+        <v>131</v>
       </c>
       <c r="M24" s="6"/>
       <c r="N24" s="58"/>
@@ -3881,27 +3839,25 @@
       <c r="Q24" s="8"/>
       <c r="S24" s="6"/>
       <c r="T24" s="58"/>
-      <c r="U24" s="106"/>
+      <c r="U24" s="105"/>
       <c r="V24" s="8"/>
       <c r="X24" s="6"/>
-      <c r="Y24" s="113"/>
-      <c r="Z24" s="114"/>
-      <c r="AA24" s="118" t="str">
+      <c r="Y24" s="110"/>
+      <c r="Z24" s="111"/>
+      <c r="AA24" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB24" s="116"/>
-      <c r="AC24" s="111"/>
-      <c r="AD24" s="117"/>
+      <c r="AB24" s="113"/>
+      <c r="AC24" s="108"/>
+      <c r="AD24" s="114"/>
       <c r="AE24" s="8"/>
       <c r="AG24" s="6"/>
-      <c r="AH24" s="108" t="s">
-        <v>130</v>
-      </c>
+      <c r="AH24" s="132"/>
       <c r="AI24" s="8"/>
     </row>
     <row r="25" spans="2:35" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B25" s="124"/>
+      <c r="B25" s="121"/>
       <c r="M25" s="6"/>
       <c r="N25" s="58"/>
       <c r="O25" s="59"/>
@@ -3912,25 +3868,25 @@
       <c r="Q25" s="8"/>
       <c r="S25" s="6"/>
       <c r="T25" s="58"/>
-      <c r="U25" s="106"/>
+      <c r="U25" s="105"/>
       <c r="V25" s="8"/>
       <c r="X25" s="6"/>
-      <c r="Y25" s="113"/>
-      <c r="Z25" s="114"/>
-      <c r="AA25" s="118" t="str">
+      <c r="Y25" s="110"/>
+      <c r="Z25" s="111"/>
+      <c r="AA25" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB25" s="116"/>
-      <c r="AC25" s="111"/>
-      <c r="AD25" s="117"/>
+      <c r="AB25" s="113"/>
+      <c r="AC25" s="108"/>
+      <c r="AD25" s="114"/>
       <c r="AE25" s="8"/>
       <c r="AG25" s="6"/>
-      <c r="AH25" s="108"/>
+      <c r="AH25" s="132"/>
       <c r="AI25" s="8"/>
     </row>
     <row r="26" spans="2:35" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B26" s="123"/>
+      <c r="B26" s="120"/>
       <c r="M26" s="6"/>
       <c r="N26" s="58"/>
       <c r="O26" s="59"/>
@@ -3941,25 +3897,25 @@
       <c r="Q26" s="8"/>
       <c r="S26" s="6"/>
       <c r="T26" s="58"/>
-      <c r="U26" s="106"/>
+      <c r="U26" s="105"/>
       <c r="V26" s="8"/>
       <c r="X26" s="6"/>
-      <c r="Y26" s="113"/>
-      <c r="Z26" s="114"/>
-      <c r="AA26" s="118" t="str">
+      <c r="Y26" s="110"/>
+      <c r="Z26" s="111"/>
+      <c r="AA26" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB26" s="116"/>
-      <c r="AC26" s="111"/>
-      <c r="AD26" s="117"/>
+      <c r="AB26" s="113"/>
+      <c r="AC26" s="108"/>
+      <c r="AD26" s="114"/>
       <c r="AE26" s="8"/>
       <c r="AG26" s="6"/>
-      <c r="AH26" s="108"/>
+      <c r="AH26" s="132"/>
       <c r="AI26" s="8"/>
     </row>
     <row r="27" spans="2:35" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B27" s="123"/>
+      <c r="B27" s="120"/>
       <c r="M27" s="6"/>
       <c r="N27" s="58"/>
       <c r="O27" s="59"/>
@@ -3970,25 +3926,25 @@
       <c r="Q27" s="8"/>
       <c r="S27" s="6"/>
       <c r="T27" s="58"/>
-      <c r="U27" s="106"/>
+      <c r="U27" s="105"/>
       <c r="V27" s="8"/>
       <c r="X27" s="6"/>
-      <c r="Y27" s="113"/>
-      <c r="Z27" s="114"/>
-      <c r="AA27" s="118" t="str">
+      <c r="Y27" s="110"/>
+      <c r="Z27" s="111"/>
+      <c r="AA27" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB27" s="116"/>
-      <c r="AC27" s="111"/>
-      <c r="AD27" s="117"/>
+      <c r="AB27" s="113"/>
+      <c r="AC27" s="108"/>
+      <c r="AD27" s="114"/>
       <c r="AE27" s="8"/>
       <c r="AG27" s="6"/>
-      <c r="AH27" s="108"/>
+      <c r="AH27" s="132"/>
       <c r="AI27" s="8"/>
     </row>
     <row r="28" spans="2:35" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B28" s="123"/>
+      <c r="B28" s="120"/>
       <c r="M28" s="6"/>
       <c r="N28" s="58"/>
       <c r="O28" s="59"/>
@@ -3999,25 +3955,25 @@
       <c r="Q28" s="8"/>
       <c r="S28" s="6"/>
       <c r="T28" s="58"/>
-      <c r="U28" s="106"/>
+      <c r="U28" s="105"/>
       <c r="V28" s="8"/>
       <c r="X28" s="6"/>
-      <c r="Y28" s="113"/>
-      <c r="Z28" s="114"/>
-      <c r="AA28" s="118" t="str">
+      <c r="Y28" s="110"/>
+      <c r="Z28" s="111"/>
+      <c r="AA28" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB28" s="116"/>
-      <c r="AC28" s="111"/>
-      <c r="AD28" s="117"/>
+      <c r="AB28" s="113"/>
+      <c r="AC28" s="108"/>
+      <c r="AD28" s="114"/>
       <c r="AE28" s="8"/>
       <c r="AG28" s="6"/>
-      <c r="AH28" s="108"/>
+      <c r="AH28" s="132"/>
       <c r="AI28" s="8"/>
     </row>
     <row r="29" spans="2:35" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="B29" s="125"/>
+      <c r="B29" s="122"/>
       <c r="M29" s="6"/>
       <c r="N29" s="58"/>
       <c r="O29" s="59"/>
@@ -4028,21 +3984,21 @@
       <c r="Q29" s="8"/>
       <c r="S29" s="6"/>
       <c r="T29" s="58"/>
-      <c r="U29" s="106"/>
+      <c r="U29" s="105"/>
       <c r="V29" s="8"/>
       <c r="X29" s="6"/>
-      <c r="Y29" s="113"/>
-      <c r="Z29" s="114"/>
-      <c r="AA29" s="118" t="str">
+      <c r="Y29" s="110"/>
+      <c r="Z29" s="111"/>
+      <c r="AA29" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB29" s="116"/>
-      <c r="AC29" s="111"/>
-      <c r="AD29" s="117"/>
+      <c r="AB29" s="113"/>
+      <c r="AC29" s="108"/>
+      <c r="AD29" s="114"/>
       <c r="AE29" s="8"/>
       <c r="AG29" s="6"/>
-      <c r="AH29" s="108"/>
+      <c r="AH29" s="132"/>
       <c r="AI29" s="8"/>
     </row>
     <row r="30" spans="2:35" x14ac:dyDescent="0.3">
@@ -4056,21 +4012,21 @@
       <c r="Q30" s="8"/>
       <c r="S30" s="6"/>
       <c r="T30" s="58"/>
-      <c r="U30" s="106"/>
+      <c r="U30" s="105"/>
       <c r="V30" s="8"/>
       <c r="X30" s="6"/>
-      <c r="Y30" s="113"/>
-      <c r="Z30" s="114"/>
-      <c r="AA30" s="118" t="str">
+      <c r="Y30" s="110"/>
+      <c r="Z30" s="111"/>
+      <c r="AA30" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB30" s="116"/>
-      <c r="AC30" s="111"/>
-      <c r="AD30" s="117"/>
+      <c r="AB30" s="113"/>
+      <c r="AC30" s="108"/>
+      <c r="AD30" s="114"/>
       <c r="AE30" s="8"/>
       <c r="AG30" s="6"/>
-      <c r="AH30" s="108"/>
+      <c r="AH30" s="132"/>
       <c r="AI30" s="8"/>
     </row>
     <row r="31" spans="2:35" x14ac:dyDescent="0.3">
@@ -4084,21 +4040,21 @@
       <c r="Q31" s="8"/>
       <c r="S31" s="6"/>
       <c r="T31" s="58"/>
-      <c r="U31" s="106"/>
+      <c r="U31" s="105"/>
       <c r="V31" s="8"/>
       <c r="X31" s="6"/>
-      <c r="Y31" s="113"/>
-      <c r="Z31" s="114"/>
-      <c r="AA31" s="118" t="str">
+      <c r="Y31" s="110"/>
+      <c r="Z31" s="111"/>
+      <c r="AA31" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB31" s="116"/>
-      <c r="AC31" s="111"/>
-      <c r="AD31" s="117"/>
+      <c r="AB31" s="113"/>
+      <c r="AC31" s="108"/>
+      <c r="AD31" s="114"/>
       <c r="AE31" s="8"/>
       <c r="AG31" s="6"/>
-      <c r="AH31" s="108"/>
+      <c r="AH31" s="132"/>
       <c r="AI31" s="8"/>
     </row>
     <row r="32" spans="2:35" x14ac:dyDescent="0.3">
@@ -4112,21 +4068,21 @@
       <c r="Q32" s="8"/>
       <c r="S32" s="6"/>
       <c r="T32" s="58"/>
-      <c r="U32" s="106"/>
+      <c r="U32" s="105"/>
       <c r="V32" s="8"/>
       <c r="X32" s="6"/>
-      <c r="Y32" s="113"/>
-      <c r="Z32" s="114"/>
-      <c r="AA32" s="118" t="str">
+      <c r="Y32" s="110"/>
+      <c r="Z32" s="111"/>
+      <c r="AA32" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB32" s="116"/>
-      <c r="AC32" s="111"/>
-      <c r="AD32" s="117"/>
+      <c r="AB32" s="113"/>
+      <c r="AC32" s="108"/>
+      <c r="AD32" s="114"/>
       <c r="AE32" s="8"/>
       <c r="AG32" s="6"/>
-      <c r="AH32" s="108"/>
+      <c r="AH32" s="132"/>
       <c r="AI32" s="8"/>
     </row>
     <row r="33" spans="13:35" x14ac:dyDescent="0.3">
@@ -4140,21 +4096,21 @@
       <c r="Q33" s="8"/>
       <c r="S33" s="6"/>
       <c r="T33" s="58"/>
-      <c r="U33" s="106"/>
+      <c r="U33" s="105"/>
       <c r="V33" s="8"/>
       <c r="X33" s="6"/>
-      <c r="Y33" s="113"/>
-      <c r="Z33" s="114"/>
-      <c r="AA33" s="118" t="str">
+      <c r="Y33" s="110"/>
+      <c r="Z33" s="111"/>
+      <c r="AA33" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB33" s="116"/>
-      <c r="AC33" s="111"/>
-      <c r="AD33" s="117"/>
+      <c r="AB33" s="113"/>
+      <c r="AC33" s="108"/>
+      <c r="AD33" s="114"/>
       <c r="AE33" s="8"/>
       <c r="AG33" s="6"/>
-      <c r="AH33" s="108"/>
+      <c r="AH33" s="132"/>
       <c r="AI33" s="8"/>
     </row>
     <row r="34" spans="13:35" x14ac:dyDescent="0.3">
@@ -4168,21 +4124,21 @@
       <c r="Q34" s="8"/>
       <c r="S34" s="6"/>
       <c r="T34" s="58"/>
-      <c r="U34" s="106"/>
+      <c r="U34" s="105"/>
       <c r="V34" s="8"/>
       <c r="X34" s="6"/>
-      <c r="Y34" s="113"/>
-      <c r="Z34" s="114"/>
-      <c r="AA34" s="118" t="str">
+      <c r="Y34" s="110"/>
+      <c r="Z34" s="111"/>
+      <c r="AA34" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB34" s="116"/>
-      <c r="AC34" s="111"/>
-      <c r="AD34" s="117"/>
+      <c r="AB34" s="113"/>
+      <c r="AC34" s="108"/>
+      <c r="AD34" s="114"/>
       <c r="AE34" s="8"/>
       <c r="AG34" s="6"/>
-      <c r="AH34" s="108"/>
+      <c r="AH34" s="132"/>
       <c r="AI34" s="8"/>
     </row>
     <row r="35" spans="13:35" x14ac:dyDescent="0.3">
@@ -4196,21 +4152,21 @@
       <c r="Q35" s="8"/>
       <c r="S35" s="6"/>
       <c r="T35" s="58"/>
-      <c r="U35" s="106"/>
+      <c r="U35" s="105"/>
       <c r="V35" s="8"/>
       <c r="X35" s="6"/>
-      <c r="Y35" s="113"/>
-      <c r="Z35" s="114"/>
-      <c r="AA35" s="118" t="str">
+      <c r="Y35" s="110"/>
+      <c r="Z35" s="111"/>
+      <c r="AA35" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB35" s="116"/>
-      <c r="AC35" s="111"/>
-      <c r="AD35" s="117"/>
+      <c r="AB35" s="113"/>
+      <c r="AC35" s="108"/>
+      <c r="AD35" s="114"/>
       <c r="AE35" s="8"/>
       <c r="AG35" s="6"/>
-      <c r="AH35" s="108"/>
+      <c r="AH35" s="132"/>
       <c r="AI35" s="8"/>
     </row>
     <row r="36" spans="13:35" x14ac:dyDescent="0.3">
@@ -4221,21 +4177,21 @@
       <c r="Q36" s="66"/>
       <c r="S36" s="6"/>
       <c r="T36" s="58"/>
-      <c r="U36" s="106"/>
+      <c r="U36" s="105"/>
       <c r="V36" s="8"/>
       <c r="X36" s="6"/>
-      <c r="Y36" s="113"/>
-      <c r="Z36" s="114"/>
-      <c r="AA36" s="118" t="str">
+      <c r="Y36" s="110"/>
+      <c r="Z36" s="111"/>
+      <c r="AA36" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB36" s="116"/>
-      <c r="AC36" s="111"/>
-      <c r="AD36" s="117"/>
+      <c r="AB36" s="113"/>
+      <c r="AC36" s="108"/>
+      <c r="AD36" s="114"/>
       <c r="AE36" s="8"/>
       <c r="AG36" s="6"/>
-      <c r="AH36" s="108"/>
+      <c r="AH36" s="132"/>
       <c r="AI36" s="8"/>
     </row>
     <row r="37" spans="13:35" x14ac:dyDescent="0.3">
@@ -4244,18 +4200,18 @@
       <c r="U37" s="60"/>
       <c r="V37" s="8"/>
       <c r="X37" s="6"/>
-      <c r="Y37" s="113"/>
-      <c r="Z37" s="114"/>
-      <c r="AA37" s="118" t="str">
+      <c r="Y37" s="110"/>
+      <c r="Z37" s="111"/>
+      <c r="AA37" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB37" s="116"/>
-      <c r="AC37" s="111"/>
-      <c r="AD37" s="117"/>
+      <c r="AB37" s="113"/>
+      <c r="AC37" s="108"/>
+      <c r="AD37" s="114"/>
       <c r="AE37" s="8"/>
       <c r="AG37" s="6"/>
-      <c r="AH37" s="108"/>
+      <c r="AH37" s="132"/>
       <c r="AI37" s="8"/>
     </row>
     <row r="38" spans="13:35" x14ac:dyDescent="0.3">
@@ -4264,18 +4220,18 @@
       <c r="U38" s="60"/>
       <c r="V38" s="8"/>
       <c r="X38" s="6"/>
-      <c r="Y38" s="113"/>
-      <c r="Z38" s="114"/>
-      <c r="AA38" s="118" t="str">
+      <c r="Y38" s="110"/>
+      <c r="Z38" s="111"/>
+      <c r="AA38" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB38" s="116"/>
-      <c r="AC38" s="111"/>
-      <c r="AD38" s="117"/>
+      <c r="AB38" s="113"/>
+      <c r="AC38" s="108"/>
+      <c r="AD38" s="114"/>
       <c r="AE38" s="8"/>
       <c r="AG38" s="6"/>
-      <c r="AH38" s="108"/>
+      <c r="AH38" s="132"/>
       <c r="AI38" s="8"/>
     </row>
     <row r="39" spans="13:35" x14ac:dyDescent="0.3">
@@ -4284,18 +4240,18 @@
       <c r="U39" s="60"/>
       <c r="V39" s="8"/>
       <c r="X39" s="6"/>
-      <c r="Y39" s="113"/>
-      <c r="Z39" s="114"/>
-      <c r="AA39" s="118" t="str">
+      <c r="Y39" s="110"/>
+      <c r="Z39" s="111"/>
+      <c r="AA39" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB39" s="116"/>
-      <c r="AC39" s="111"/>
-      <c r="AD39" s="117"/>
+      <c r="AB39" s="113"/>
+      <c r="AC39" s="108"/>
+      <c r="AD39" s="114"/>
       <c r="AE39" s="8"/>
       <c r="AG39" s="6"/>
-      <c r="AH39" s="108"/>
+      <c r="AH39" s="132"/>
       <c r="AI39" s="8"/>
     </row>
     <row r="40" spans="13:35" x14ac:dyDescent="0.3">
@@ -4304,18 +4260,18 @@
       <c r="U40" s="60"/>
       <c r="V40" s="8"/>
       <c r="X40" s="6"/>
-      <c r="Y40" s="113"/>
-      <c r="Z40" s="114"/>
-      <c r="AA40" s="118" t="str">
+      <c r="Y40" s="110"/>
+      <c r="Z40" s="111"/>
+      <c r="AA40" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB40" s="116"/>
-      <c r="AC40" s="111"/>
-      <c r="AD40" s="117"/>
+      <c r="AB40" s="113"/>
+      <c r="AC40" s="108"/>
+      <c r="AD40" s="114"/>
       <c r="AE40" s="8"/>
       <c r="AG40" s="6"/>
-      <c r="AH40" s="108"/>
+      <c r="AH40" s="132"/>
       <c r="AI40" s="8"/>
     </row>
     <row r="41" spans="13:35" x14ac:dyDescent="0.3">
@@ -4324,18 +4280,18 @@
       <c r="U41" s="60"/>
       <c r="V41" s="8"/>
       <c r="X41" s="6"/>
-      <c r="Y41" s="113"/>
-      <c r="Z41" s="114"/>
-      <c r="AA41" s="118" t="str">
+      <c r="Y41" s="110"/>
+      <c r="Z41" s="111"/>
+      <c r="AA41" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB41" s="116"/>
-      <c r="AC41" s="111"/>
-      <c r="AD41" s="117"/>
+      <c r="AB41" s="113"/>
+      <c r="AC41" s="108"/>
+      <c r="AD41" s="114"/>
       <c r="AE41" s="8"/>
       <c r="AG41" s="6"/>
-      <c r="AH41" s="108"/>
+      <c r="AH41" s="132"/>
       <c r="AI41" s="8"/>
     </row>
     <row r="42" spans="13:35" x14ac:dyDescent="0.3">
@@ -4344,18 +4300,18 @@
       <c r="U42" s="60"/>
       <c r="V42" s="8"/>
       <c r="X42" s="6"/>
-      <c r="Y42" s="113"/>
-      <c r="Z42" s="114"/>
-      <c r="AA42" s="118" t="str">
+      <c r="Y42" s="110"/>
+      <c r="Z42" s="111"/>
+      <c r="AA42" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB42" s="116"/>
-      <c r="AC42" s="111"/>
-      <c r="AD42" s="117"/>
+      <c r="AB42" s="113"/>
+      <c r="AC42" s="108"/>
+      <c r="AD42" s="114"/>
       <c r="AE42" s="8"/>
       <c r="AG42" s="6"/>
-      <c r="AH42" s="108"/>
+      <c r="AH42" s="132"/>
       <c r="AI42" s="8"/>
     </row>
     <row r="43" spans="13:35" x14ac:dyDescent="0.3">
@@ -4364,18 +4320,18 @@
       <c r="U43" s="60"/>
       <c r="V43" s="8"/>
       <c r="X43" s="6"/>
-      <c r="Y43" s="113"/>
-      <c r="Z43" s="114"/>
-      <c r="AA43" s="118" t="str">
+      <c r="Y43" s="110"/>
+      <c r="Z43" s="111"/>
+      <c r="AA43" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB43" s="116"/>
-      <c r="AC43" s="111"/>
-      <c r="AD43" s="117"/>
+      <c r="AB43" s="113"/>
+      <c r="AC43" s="108"/>
+      <c r="AD43" s="114"/>
       <c r="AE43" s="8"/>
       <c r="AG43" s="6"/>
-      <c r="AH43" s="108"/>
+      <c r="AH43" s="132"/>
       <c r="AI43" s="8"/>
     </row>
     <row r="44" spans="13:35" x14ac:dyDescent="0.3">
@@ -4384,18 +4340,18 @@
       <c r="U44" s="60"/>
       <c r="V44" s="8"/>
       <c r="X44" s="6"/>
-      <c r="Y44" s="113"/>
-      <c r="Z44" s="114"/>
-      <c r="AA44" s="118" t="str">
+      <c r="Y44" s="110"/>
+      <c r="Z44" s="111"/>
+      <c r="AA44" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB44" s="116"/>
-      <c r="AC44" s="111"/>
-      <c r="AD44" s="117"/>
+      <c r="AB44" s="113"/>
+      <c r="AC44" s="108"/>
+      <c r="AD44" s="114"/>
       <c r="AE44" s="8"/>
       <c r="AG44" s="6"/>
-      <c r="AH44" s="108"/>
+      <c r="AH44" s="132"/>
       <c r="AI44" s="8"/>
     </row>
     <row r="45" spans="13:35" x14ac:dyDescent="0.3">
@@ -4404,18 +4360,18 @@
       <c r="U45" s="60"/>
       <c r="V45" s="8"/>
       <c r="X45" s="6"/>
-      <c r="Y45" s="113"/>
-      <c r="Z45" s="114"/>
-      <c r="AA45" s="118" t="str">
+      <c r="Y45" s="110"/>
+      <c r="Z45" s="111"/>
+      <c r="AA45" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB45" s="116"/>
-      <c r="AC45" s="111"/>
-      <c r="AD45" s="117"/>
+      <c r="AB45" s="113"/>
+      <c r="AC45" s="108"/>
+      <c r="AD45" s="114"/>
       <c r="AE45" s="8"/>
       <c r="AG45" s="6"/>
-      <c r="AH45" s="108"/>
+      <c r="AH45" s="132"/>
       <c r="AI45" s="8"/>
     </row>
     <row r="46" spans="13:35" x14ac:dyDescent="0.3">
@@ -4424,18 +4380,18 @@
       <c r="U46" s="60"/>
       <c r="V46" s="8"/>
       <c r="X46" s="6"/>
-      <c r="Y46" s="113"/>
-      <c r="Z46" s="114"/>
-      <c r="AA46" s="118" t="str">
+      <c r="Y46" s="110"/>
+      <c r="Z46" s="111"/>
+      <c r="AA46" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB46" s="116"/>
-      <c r="AC46" s="111"/>
-      <c r="AD46" s="117"/>
+      <c r="AB46" s="113"/>
+      <c r="AC46" s="108"/>
+      <c r="AD46" s="114"/>
       <c r="AE46" s="8"/>
       <c r="AG46" s="6"/>
-      <c r="AH46" s="108"/>
+      <c r="AH46" s="132"/>
       <c r="AI46" s="8"/>
     </row>
     <row r="47" spans="13:35" x14ac:dyDescent="0.3">
@@ -4444,18 +4400,18 @@
       <c r="U47" s="60"/>
       <c r="V47" s="8"/>
       <c r="X47" s="6"/>
-      <c r="Y47" s="113"/>
-      <c r="Z47" s="114"/>
-      <c r="AA47" s="118" t="str">
+      <c r="Y47" s="110"/>
+      <c r="Z47" s="111"/>
+      <c r="AA47" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB47" s="116"/>
-      <c r="AC47" s="111"/>
-      <c r="AD47" s="117"/>
+      <c r="AB47" s="113"/>
+      <c r="AC47" s="108"/>
+      <c r="AD47" s="114"/>
       <c r="AE47" s="8"/>
       <c r="AG47" s="6"/>
-      <c r="AH47" s="108"/>
+      <c r="AH47" s="132"/>
       <c r="AI47" s="8"/>
     </row>
     <row r="48" spans="13:35" x14ac:dyDescent="0.3">
@@ -4464,18 +4420,18 @@
       <c r="U48" s="60"/>
       <c r="V48" s="8"/>
       <c r="X48" s="6"/>
-      <c r="Y48" s="113"/>
-      <c r="Z48" s="114"/>
-      <c r="AA48" s="118" t="str">
+      <c r="Y48" s="110"/>
+      <c r="Z48" s="111"/>
+      <c r="AA48" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB48" s="116"/>
-      <c r="AC48" s="111"/>
-      <c r="AD48" s="117"/>
+      <c r="AB48" s="113"/>
+      <c r="AC48" s="108"/>
+      <c r="AD48" s="114"/>
       <c r="AE48" s="8"/>
       <c r="AG48" s="6"/>
-      <c r="AH48" s="108"/>
+      <c r="AH48" s="132"/>
       <c r="AI48" s="8"/>
     </row>
     <row r="49" spans="19:35" x14ac:dyDescent="0.3">
@@ -4484,18 +4440,18 @@
       <c r="U49" s="60"/>
       <c r="V49" s="8"/>
       <c r="X49" s="6"/>
-      <c r="Y49" s="113"/>
-      <c r="Z49" s="114"/>
-      <c r="AA49" s="118" t="str">
+      <c r="Y49" s="110"/>
+      <c r="Z49" s="111"/>
+      <c r="AA49" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB49" s="116"/>
-      <c r="AC49" s="111"/>
-      <c r="AD49" s="117"/>
+      <c r="AB49" s="113"/>
+      <c r="AC49" s="108"/>
+      <c r="AD49" s="114"/>
       <c r="AE49" s="8"/>
       <c r="AG49" s="6"/>
-      <c r="AH49" s="108"/>
+      <c r="AH49" s="132"/>
       <c r="AI49" s="8"/>
     </row>
     <row r="50" spans="19:35" x14ac:dyDescent="0.3">
@@ -4504,18 +4460,18 @@
       <c r="U50" s="60"/>
       <c r="V50" s="8"/>
       <c r="X50" s="6"/>
-      <c r="Y50" s="113"/>
-      <c r="Z50" s="114"/>
-      <c r="AA50" s="118" t="str">
+      <c r="Y50" s="110"/>
+      <c r="Z50" s="111"/>
+      <c r="AA50" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB50" s="116"/>
-      <c r="AC50" s="111"/>
-      <c r="AD50" s="117"/>
+      <c r="AB50" s="113"/>
+      <c r="AC50" s="108"/>
+      <c r="AD50" s="114"/>
       <c r="AE50" s="8"/>
       <c r="AG50" s="6"/>
-      <c r="AH50" s="108"/>
+      <c r="AH50" s="132"/>
       <c r="AI50" s="8"/>
     </row>
     <row r="51" spans="19:35" x14ac:dyDescent="0.3">
@@ -4524,18 +4480,18 @@
       <c r="U51" s="60"/>
       <c r="V51" s="8"/>
       <c r="X51" s="6"/>
-      <c r="Y51" s="113"/>
-      <c r="Z51" s="114"/>
-      <c r="AA51" s="118" t="str">
+      <c r="Y51" s="110"/>
+      <c r="Z51" s="111"/>
+      <c r="AA51" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB51" s="116"/>
-      <c r="AC51" s="111"/>
-      <c r="AD51" s="117"/>
+      <c r="AB51" s="113"/>
+      <c r="AC51" s="108"/>
+      <c r="AD51" s="114"/>
       <c r="AE51" s="8"/>
       <c r="AG51" s="6"/>
-      <c r="AH51" s="108"/>
+      <c r="AH51" s="132"/>
       <c r="AI51" s="8"/>
     </row>
     <row r="52" spans="19:35" x14ac:dyDescent="0.3">
@@ -4544,18 +4500,18 @@
       <c r="U52" s="60"/>
       <c r="V52" s="8"/>
       <c r="X52" s="6"/>
-      <c r="Y52" s="113"/>
-      <c r="Z52" s="114"/>
-      <c r="AA52" s="118" t="str">
+      <c r="Y52" s="110"/>
+      <c r="Z52" s="111"/>
+      <c r="AA52" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB52" s="116"/>
-      <c r="AC52" s="111"/>
-      <c r="AD52" s="117"/>
+      <c r="AB52" s="113"/>
+      <c r="AC52" s="108"/>
+      <c r="AD52" s="114"/>
       <c r="AE52" s="8"/>
       <c r="AG52" s="6"/>
-      <c r="AH52" s="108"/>
+      <c r="AH52" s="132"/>
       <c r="AI52" s="8"/>
     </row>
     <row r="53" spans="19:35" x14ac:dyDescent="0.3">
@@ -4564,18 +4520,18 @@
       <c r="U53" s="60"/>
       <c r="V53" s="8"/>
       <c r="X53" s="6"/>
-      <c r="Y53" s="113"/>
-      <c r="Z53" s="114"/>
-      <c r="AA53" s="118" t="str">
+      <c r="Y53" s="110"/>
+      <c r="Z53" s="111"/>
+      <c r="AA53" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB53" s="116"/>
-      <c r="AC53" s="111"/>
-      <c r="AD53" s="117"/>
+      <c r="AB53" s="113"/>
+      <c r="AC53" s="108"/>
+      <c r="AD53" s="114"/>
       <c r="AE53" s="8"/>
       <c r="AG53" s="6"/>
-      <c r="AH53" s="108"/>
+      <c r="AH53" s="132"/>
       <c r="AI53" s="8"/>
     </row>
     <row r="54" spans="19:35" x14ac:dyDescent="0.3">
@@ -4584,82 +4540,82 @@
       <c r="U54" s="11"/>
       <c r="V54" s="12"/>
       <c r="X54" s="6"/>
-      <c r="Y54" s="113"/>
-      <c r="Z54" s="114"/>
-      <c r="AA54" s="118" t="str">
+      <c r="Y54" s="110"/>
+      <c r="Z54" s="111"/>
+      <c r="AA54" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB54" s="116"/>
-      <c r="AC54" s="111"/>
-      <c r="AD54" s="117"/>
+      <c r="AB54" s="113"/>
+      <c r="AC54" s="108"/>
+      <c r="AD54" s="114"/>
       <c r="AE54" s="8"/>
       <c r="AG54" s="6"/>
-      <c r="AH54" s="108"/>
+      <c r="AH54" s="132"/>
       <c r="AI54" s="8"/>
     </row>
     <row r="55" spans="19:35" x14ac:dyDescent="0.3">
       <c r="X55" s="6"/>
-      <c r="Y55" s="113"/>
-      <c r="Z55" s="114"/>
-      <c r="AA55" s="118" t="str">
+      <c r="Y55" s="110"/>
+      <c r="Z55" s="111"/>
+      <c r="AA55" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB55" s="116"/>
-      <c r="AC55" s="111"/>
-      <c r="AD55" s="117"/>
+      <c r="AB55" s="113"/>
+      <c r="AC55" s="108"/>
+      <c r="AD55" s="114"/>
       <c r="AE55" s="8"/>
       <c r="AG55" s="6"/>
-      <c r="AH55" s="108"/>
+      <c r="AH55" s="132"/>
       <c r="AI55" s="8"/>
     </row>
     <row r="56" spans="19:35" x14ac:dyDescent="0.3">
       <c r="X56" s="6"/>
-      <c r="Y56" s="113"/>
-      <c r="Z56" s="114"/>
-      <c r="AA56" s="118" t="str">
+      <c r="Y56" s="110"/>
+      <c r="Z56" s="111"/>
+      <c r="AA56" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB56" s="116"/>
-      <c r="AC56" s="111"/>
-      <c r="AD56" s="117"/>
+      <c r="AB56" s="113"/>
+      <c r="AC56" s="108"/>
+      <c r="AD56" s="114"/>
       <c r="AE56" s="8"/>
       <c r="AG56" s="6"/>
-      <c r="AH56" s="108"/>
+      <c r="AH56" s="132"/>
       <c r="AI56" s="8"/>
     </row>
     <row r="57" spans="19:35" x14ac:dyDescent="0.3">
       <c r="X57" s="6"/>
-      <c r="Y57" s="113"/>
-      <c r="Z57" s="114"/>
-      <c r="AA57" s="118" t="str">
+      <c r="Y57" s="110"/>
+      <c r="Z57" s="111"/>
+      <c r="AA57" s="115" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB57" s="116"/>
-      <c r="AC57" s="111"/>
-      <c r="AD57" s="117"/>
+      <c r="AB57" s="113"/>
+      <c r="AC57" s="108"/>
+      <c r="AD57" s="114"/>
       <c r="AE57" s="8"/>
       <c r="AG57" s="6"/>
-      <c r="AH57" s="108"/>
+      <c r="AH57" s="132"/>
       <c r="AI57" s="8"/>
     </row>
     <row r="58" spans="19:35" x14ac:dyDescent="0.3">
       <c r="X58" s="6"/>
-      <c r="Y58" s="113"/>
-      <c r="Z58" s="119"/>
-      <c r="AA58" s="120" t="str">
+      <c r="Y58" s="110"/>
+      <c r="Z58" s="116"/>
+      <c r="AA58" s="117" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AB58" s="116"/>
-      <c r="AC58" s="111"/>
-      <c r="AD58" s="117"/>
+      <c r="AB58" s="113"/>
+      <c r="AC58" s="108"/>
+      <c r="AD58" s="114"/>
       <c r="AE58" s="8"/>
       <c r="AG58" s="6"/>
-      <c r="AH58" s="108"/>
+      <c r="AH58" s="132"/>
       <c r="AI58" s="8"/>
     </row>
     <row r="59" spans="19:35" x14ac:dyDescent="0.3">
@@ -4667,783 +4623,783 @@
       <c r="Y59" s="11"/>
       <c r="Z59" s="11"/>
       <c r="AA59" s="11"/>
-      <c r="AB59" s="121"/>
-      <c r="AC59" s="121"/>
+      <c r="AB59" s="118"/>
+      <c r="AC59" s="118"/>
       <c r="AD59" s="11"/>
       <c r="AE59" s="12"/>
       <c r="AG59" s="6"/>
-      <c r="AH59" s="108"/>
+      <c r="AH59" s="132"/>
       <c r="AI59" s="8"/>
     </row>
     <row r="60" spans="19:35" x14ac:dyDescent="0.3">
       <c r="AG60" s="6"/>
-      <c r="AH60" s="108"/>
+      <c r="AH60" s="132"/>
       <c r="AI60" s="8"/>
     </row>
     <row r="61" spans="19:35" x14ac:dyDescent="0.3">
-      <c r="Y61" s="122"/>
+      <c r="Y61" s="119"/>
       <c r="AG61" s="6"/>
-      <c r="AH61" s="108"/>
+      <c r="AH61" s="132"/>
       <c r="AI61" s="8"/>
     </row>
     <row r="62" spans="19:35" x14ac:dyDescent="0.3">
-      <c r="Y62" s="122"/>
-      <c r="Z62" s="122"/>
-      <c r="AA62" s="122"/>
+      <c r="Y62" s="119"/>
+      <c r="Z62" s="119"/>
+      <c r="AA62" s="119"/>
       <c r="AG62" s="6"/>
-      <c r="AH62" s="108"/>
+      <c r="AH62" s="132"/>
       <c r="AI62" s="8"/>
     </row>
     <row r="63" spans="19:35" x14ac:dyDescent="0.3">
-      <c r="Y63" s="122"/>
-      <c r="Z63" s="122"/>
-      <c r="AA63" s="122"/>
+      <c r="Y63" s="119"/>
+      <c r="Z63" s="119"/>
+      <c r="AA63" s="119"/>
       <c r="AG63" s="6"/>
-      <c r="AH63" s="108"/>
+      <c r="AH63" s="132"/>
       <c r="AI63" s="8"/>
     </row>
     <row r="64" spans="19:35" x14ac:dyDescent="0.3">
-      <c r="Y64" s="122"/>
-      <c r="Z64" s="122"/>
-      <c r="AA64" s="122"/>
+      <c r="Y64" s="119"/>
+      <c r="Z64" s="119"/>
+      <c r="AA64" s="119"/>
       <c r="AG64" s="6"/>
-      <c r="AH64" s="108"/>
+      <c r="AH64" s="132"/>
       <c r="AI64" s="8"/>
     </row>
     <row r="65" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y65" s="122"/>
-      <c r="Z65" s="122"/>
-      <c r="AA65" s="122"/>
+      <c r="Y65" s="119"/>
+      <c r="Z65" s="119"/>
+      <c r="AA65" s="119"/>
       <c r="AG65" s="6"/>
-      <c r="AH65" s="108"/>
+      <c r="AH65" s="132"/>
       <c r="AI65" s="8"/>
     </row>
     <row r="66" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y66" s="122"/>
-      <c r="Z66" s="122"/>
-      <c r="AA66" s="122"/>
+      <c r="Y66" s="119"/>
+      <c r="Z66" s="119"/>
+      <c r="AA66" s="119"/>
       <c r="AG66" s="6"/>
-      <c r="AH66" s="108"/>
+      <c r="AH66" s="132"/>
       <c r="AI66" s="8"/>
     </row>
     <row r="67" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y67" s="122"/>
-      <c r="Z67" s="122"/>
-      <c r="AA67" s="122"/>
+      <c r="Y67" s="119"/>
+      <c r="Z67" s="119"/>
+      <c r="AA67" s="119"/>
       <c r="AG67" s="6"/>
-      <c r="AH67" s="108"/>
+      <c r="AH67" s="132"/>
       <c r="AI67" s="8"/>
     </row>
     <row r="68" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y68" s="122"/>
-      <c r="Z68" s="122"/>
-      <c r="AA68" s="122"/>
+      <c r="Y68" s="119"/>
+      <c r="Z68" s="119"/>
+      <c r="AA68" s="119"/>
       <c r="AG68" s="6"/>
-      <c r="AH68" s="108"/>
+      <c r="AH68" s="132"/>
       <c r="AI68" s="8"/>
     </row>
     <row r="69" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y69" s="122"/>
-      <c r="Z69" s="122"/>
-      <c r="AA69" s="122"/>
+      <c r="Y69" s="119"/>
+      <c r="Z69" s="119"/>
+      <c r="AA69" s="119"/>
       <c r="AG69" s="6"/>
-      <c r="AH69" s="108"/>
+      <c r="AH69" s="132"/>
       <c r="AI69" s="8"/>
     </row>
     <row r="70" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y70" s="122"/>
-      <c r="Z70" s="122"/>
-      <c r="AA70" s="122"/>
+      <c r="Y70" s="119"/>
+      <c r="Z70" s="119"/>
+      <c r="AA70" s="119"/>
       <c r="AG70" s="6"/>
-      <c r="AH70" s="108"/>
+      <c r="AH70" s="132"/>
       <c r="AI70" s="8"/>
     </row>
     <row r="71" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y71" s="122"/>
-      <c r="Z71" s="122"/>
-      <c r="AA71" s="122"/>
+      <c r="Y71" s="119"/>
+      <c r="Z71" s="119"/>
+      <c r="AA71" s="119"/>
       <c r="AG71" s="6"/>
-      <c r="AH71" s="108"/>
+      <c r="AH71" s="132"/>
       <c r="AI71" s="8"/>
     </row>
     <row r="72" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y72" s="122"/>
-      <c r="Z72" s="122"/>
-      <c r="AA72" s="122"/>
+      <c r="Y72" s="119"/>
+      <c r="Z72" s="119"/>
+      <c r="AA72" s="119"/>
       <c r="AG72" s="6"/>
-      <c r="AH72" s="108"/>
+      <c r="AH72" s="132"/>
       <c r="AI72" s="8"/>
     </row>
     <row r="73" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y73" s="122"/>
-      <c r="Z73" s="122"/>
-      <c r="AA73" s="122"/>
+      <c r="Y73" s="119"/>
+      <c r="Z73" s="119"/>
+      <c r="AA73" s="119"/>
       <c r="AG73" s="6"/>
-      <c r="AH73" s="108"/>
+      <c r="AH73" s="132"/>
       <c r="AI73" s="8"/>
     </row>
     <row r="74" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y74" s="122"/>
-      <c r="Z74" s="122"/>
-      <c r="AA74" s="122"/>
+      <c r="Y74" s="119"/>
+      <c r="Z74" s="119"/>
+      <c r="AA74" s="119"/>
       <c r="AG74" s="6"/>
-      <c r="AH74" s="108"/>
+      <c r="AH74" s="132"/>
       <c r="AI74" s="8"/>
     </row>
     <row r="75" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y75" s="122"/>
+      <c r="Y75" s="119"/>
       <c r="AG75" s="6"/>
-      <c r="AH75" s="108"/>
+      <c r="AH75" s="132"/>
       <c r="AI75" s="8"/>
     </row>
     <row r="76" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y76" s="122"/>
+      <c r="Y76" s="119"/>
       <c r="AG76" s="6"/>
-      <c r="AH76" s="108"/>
+      <c r="AH76" s="132"/>
       <c r="AI76" s="8"/>
     </row>
     <row r="77" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y77" s="122"/>
+      <c r="Y77" s="119"/>
       <c r="AG77" s="6"/>
-      <c r="AH77" s="108"/>
+      <c r="AH77" s="132"/>
       <c r="AI77" s="8"/>
     </row>
     <row r="78" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y78" s="122"/>
+      <c r="Y78" s="119"/>
       <c r="AG78" s="6"/>
-      <c r="AH78" s="108"/>
+      <c r="AH78" s="132"/>
       <c r="AI78" s="8"/>
     </row>
     <row r="79" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y79" s="122"/>
+      <c r="Y79" s="119"/>
       <c r="AG79" s="6"/>
-      <c r="AH79" s="108"/>
+      <c r="AH79" s="132"/>
       <c r="AI79" s="8"/>
     </row>
     <row r="80" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y80" s="122"/>
+      <c r="Y80" s="119"/>
       <c r="AG80" s="6"/>
-      <c r="AH80" s="108"/>
+      <c r="AH80" s="132"/>
       <c r="AI80" s="8"/>
     </row>
     <row r="81" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y81" s="122"/>
+      <c r="Y81" s="119"/>
       <c r="AG81" s="6"/>
-      <c r="AH81" s="108"/>
+      <c r="AH81" s="132"/>
       <c r="AI81" s="8"/>
     </row>
     <row r="82" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y82" s="122"/>
+      <c r="Y82" s="119"/>
       <c r="AG82" s="6"/>
-      <c r="AH82" s="108"/>
+      <c r="AH82" s="132"/>
       <c r="AI82" s="8"/>
     </row>
     <row r="83" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y83" s="122"/>
+      <c r="Y83" s="119"/>
       <c r="AG83" s="6"/>
-      <c r="AH83" s="108"/>
+      <c r="AH83" s="132"/>
       <c r="AI83" s="8"/>
     </row>
     <row r="84" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y84" s="122"/>
+      <c r="Y84" s="119"/>
       <c r="AG84" s="6"/>
-      <c r="AH84" s="108"/>
+      <c r="AH84" s="132"/>
       <c r="AI84" s="8"/>
     </row>
     <row r="85" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y85" s="122"/>
+      <c r="Y85" s="119"/>
       <c r="AG85" s="6"/>
-      <c r="AH85" s="108"/>
+      <c r="AH85" s="132"/>
       <c r="AI85" s="8"/>
     </row>
     <row r="86" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y86" s="122"/>
+      <c r="Y86" s="119"/>
       <c r="AG86" s="6"/>
-      <c r="AH86" s="108"/>
+      <c r="AH86" s="132"/>
       <c r="AI86" s="8"/>
     </row>
     <row r="87" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y87" s="122"/>
+      <c r="Y87" s="119"/>
       <c r="AG87" s="6"/>
-      <c r="AH87" s="108"/>
+      <c r="AH87" s="132"/>
       <c r="AI87" s="8"/>
     </row>
     <row r="88" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y88" s="122"/>
+      <c r="Y88" s="119"/>
       <c r="AG88" s="6"/>
-      <c r="AH88" s="108"/>
+      <c r="AH88" s="132"/>
       <c r="AI88" s="8"/>
     </row>
     <row r="89" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y89" s="122"/>
+      <c r="Y89" s="119"/>
       <c r="AG89" s="6"/>
-      <c r="AH89" s="108"/>
+      <c r="AH89" s="132"/>
       <c r="AI89" s="8"/>
     </row>
     <row r="90" spans="25:35" x14ac:dyDescent="0.3">
-      <c r="Y90" s="122"/>
+      <c r="Y90" s="119"/>
       <c r="AG90" s="6"/>
-      <c r="AH90" s="108"/>
+      <c r="AH90" s="132"/>
       <c r="AI90" s="8"/>
     </row>
     <row r="91" spans="25:35" x14ac:dyDescent="0.3">
       <c r="AG91" s="6"/>
-      <c r="AH91" s="108"/>
+      <c r="AH91" s="132"/>
       <c r="AI91" s="8"/>
     </row>
     <row r="92" spans="25:35" x14ac:dyDescent="0.3">
       <c r="AG92" s="6"/>
-      <c r="AH92" s="108"/>
+      <c r="AH92" s="132"/>
       <c r="AI92" s="8"/>
     </row>
     <row r="93" spans="25:35" x14ac:dyDescent="0.3">
       <c r="AG93" s="6"/>
-      <c r="AH93" s="108"/>
+      <c r="AH93" s="132"/>
       <c r="AI93" s="8"/>
     </row>
     <row r="94" spans="25:35" x14ac:dyDescent="0.3">
       <c r="AG94" s="6"/>
-      <c r="AH94" s="108"/>
+      <c r="AH94" s="132"/>
       <c r="AI94" s="8"/>
     </row>
     <row r="95" spans="25:35" x14ac:dyDescent="0.3">
       <c r="AG95" s="6"/>
-      <c r="AH95" s="108"/>
+      <c r="AH95" s="132"/>
       <c r="AI95" s="8"/>
     </row>
     <row r="96" spans="25:35" x14ac:dyDescent="0.3">
       <c r="AG96" s="6"/>
-      <c r="AH96" s="108"/>
+      <c r="AH96" s="132"/>
       <c r="AI96" s="8"/>
     </row>
     <row r="97" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG97" s="6"/>
-      <c r="AH97" s="108"/>
+      <c r="AH97" s="132"/>
       <c r="AI97" s="8"/>
     </row>
     <row r="98" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG98" s="6"/>
-      <c r="AH98" s="108"/>
+      <c r="AH98" s="132"/>
       <c r="AI98" s="8"/>
     </row>
     <row r="99" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG99" s="6"/>
-      <c r="AH99" s="108"/>
+      <c r="AH99" s="132"/>
       <c r="AI99" s="8"/>
     </row>
     <row r="100" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG100" s="6"/>
-      <c r="AH100" s="108"/>
+      <c r="AH100" s="132"/>
       <c r="AI100" s="8"/>
     </row>
     <row r="101" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG101" s="6"/>
-      <c r="AH101" s="108"/>
+      <c r="AH101" s="132"/>
       <c r="AI101" s="8"/>
     </row>
     <row r="102" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG102" s="6"/>
-      <c r="AH102" s="108"/>
+      <c r="AH102" s="132"/>
       <c r="AI102" s="8"/>
     </row>
     <row r="103" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG103" s="6"/>
-      <c r="AH103" s="108"/>
+      <c r="AH103" s="132"/>
       <c r="AI103" s="8"/>
     </row>
     <row r="104" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG104" s="6"/>
-      <c r="AH104" s="108"/>
+      <c r="AH104" s="132"/>
       <c r="AI104" s="8"/>
     </row>
     <row r="105" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG105" s="6"/>
-      <c r="AH105" s="108"/>
+      <c r="AH105" s="132"/>
       <c r="AI105" s="8"/>
     </row>
     <row r="106" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG106" s="6"/>
-      <c r="AH106" s="108"/>
+      <c r="AH106" s="132"/>
       <c r="AI106" s="8"/>
     </row>
     <row r="107" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG107" s="6"/>
-      <c r="AH107" s="108"/>
+      <c r="AH107" s="132"/>
       <c r="AI107" s="8"/>
     </row>
     <row r="108" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG108" s="6"/>
-      <c r="AH108" s="108"/>
+      <c r="AH108" s="132"/>
       <c r="AI108" s="8"/>
     </row>
     <row r="109" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG109" s="6"/>
-      <c r="AH109" s="108"/>
+      <c r="AH109" s="132"/>
       <c r="AI109" s="8"/>
     </row>
     <row r="110" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG110" s="6"/>
-      <c r="AH110" s="108"/>
+      <c r="AH110" s="132"/>
       <c r="AI110" s="8"/>
     </row>
     <row r="111" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG111" s="6"/>
-      <c r="AH111" s="108"/>
+      <c r="AH111" s="132"/>
       <c r="AI111" s="8"/>
     </row>
     <row r="112" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG112" s="6"/>
-      <c r="AH112" s="108"/>
+      <c r="AH112" s="132"/>
       <c r="AI112" s="8"/>
     </row>
     <row r="113" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG113" s="6"/>
-      <c r="AH113" s="108"/>
+      <c r="AH113" s="132"/>
       <c r="AI113" s="8"/>
     </row>
     <row r="114" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG114" s="6"/>
-      <c r="AH114" s="108"/>
+      <c r="AH114" s="132"/>
       <c r="AI114" s="8"/>
     </row>
     <row r="115" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG115" s="6"/>
-      <c r="AH115" s="108"/>
+      <c r="AH115" s="132"/>
       <c r="AI115" s="8"/>
     </row>
     <row r="116" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG116" s="6"/>
-      <c r="AH116" s="108"/>
+      <c r="AH116" s="132"/>
       <c r="AI116" s="8"/>
     </row>
     <row r="117" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG117" s="6"/>
-      <c r="AH117" s="108"/>
+      <c r="AH117" s="132"/>
       <c r="AI117" s="8"/>
     </row>
     <row r="118" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG118" s="6"/>
-      <c r="AH118" s="108"/>
+      <c r="AH118" s="132"/>
       <c r="AI118" s="8"/>
     </row>
     <row r="119" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG119" s="6"/>
-      <c r="AH119" s="108"/>
+      <c r="AH119" s="132"/>
       <c r="AI119" s="8"/>
     </row>
     <row r="120" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG120" s="6"/>
-      <c r="AH120" s="108"/>
+      <c r="AH120" s="132"/>
       <c r="AI120" s="8"/>
     </row>
     <row r="121" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG121" s="6"/>
-      <c r="AH121" s="108"/>
+      <c r="AH121" s="132"/>
       <c r="AI121" s="8"/>
     </row>
     <row r="122" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG122" s="6"/>
-      <c r="AH122" s="108"/>
+      <c r="AH122" s="132"/>
       <c r="AI122" s="8"/>
     </row>
     <row r="123" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG123" s="6"/>
-      <c r="AH123" s="108"/>
+      <c r="AH123" s="132"/>
       <c r="AI123" s="8"/>
     </row>
     <row r="124" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG124" s="6"/>
-      <c r="AH124" s="108"/>
+      <c r="AH124" s="132"/>
       <c r="AI124" s="8"/>
     </row>
     <row r="125" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG125" s="6"/>
-      <c r="AH125" s="108"/>
+      <c r="AH125" s="132"/>
       <c r="AI125" s="8"/>
     </row>
     <row r="126" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG126" s="6"/>
-      <c r="AH126" s="108"/>
+      <c r="AH126" s="132"/>
       <c r="AI126" s="8"/>
     </row>
     <row r="127" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG127" s="6"/>
-      <c r="AH127" s="108"/>
+      <c r="AH127" s="132"/>
       <c r="AI127" s="8"/>
     </row>
     <row r="128" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG128" s="6"/>
-      <c r="AH128" s="108"/>
+      <c r="AH128" s="132"/>
       <c r="AI128" s="8"/>
     </row>
     <row r="129" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG129" s="6"/>
-      <c r="AH129" s="108"/>
+      <c r="AH129" s="132"/>
       <c r="AI129" s="8"/>
     </row>
     <row r="130" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG130" s="6"/>
-      <c r="AH130" s="108"/>
+      <c r="AH130" s="132"/>
       <c r="AI130" s="8"/>
     </row>
     <row r="131" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG131" s="6"/>
-      <c r="AH131" s="108"/>
+      <c r="AH131" s="132"/>
       <c r="AI131" s="8"/>
     </row>
     <row r="132" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG132" s="6"/>
-      <c r="AH132" s="108"/>
+      <c r="AH132" s="132"/>
       <c r="AI132" s="8"/>
     </row>
     <row r="133" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG133" s="6"/>
-      <c r="AH133" s="108"/>
+      <c r="AH133" s="132"/>
       <c r="AI133" s="8"/>
     </row>
     <row r="134" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG134" s="6"/>
-      <c r="AH134" s="108"/>
+      <c r="AH134" s="132"/>
       <c r="AI134" s="8"/>
     </row>
     <row r="135" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG135" s="6"/>
-      <c r="AH135" s="108"/>
+      <c r="AH135" s="132"/>
       <c r="AI135" s="8"/>
     </row>
     <row r="136" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG136" s="6"/>
-      <c r="AH136" s="108"/>
+      <c r="AH136" s="132"/>
       <c r="AI136" s="8"/>
     </row>
     <row r="137" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG137" s="6"/>
-      <c r="AH137" s="108"/>
+      <c r="AH137" s="132"/>
       <c r="AI137" s="8"/>
     </row>
     <row r="138" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG138" s="6"/>
-      <c r="AH138" s="108"/>
+      <c r="AH138" s="132"/>
       <c r="AI138" s="8"/>
     </row>
     <row r="139" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG139" s="6"/>
-      <c r="AH139" s="108"/>
+      <c r="AH139" s="132"/>
       <c r="AI139" s="8"/>
     </row>
     <row r="140" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG140" s="6"/>
-      <c r="AH140" s="108"/>
+      <c r="AH140" s="132"/>
       <c r="AI140" s="8"/>
     </row>
     <row r="141" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG141" s="6"/>
-      <c r="AH141" s="108"/>
+      <c r="AH141" s="132"/>
       <c r="AI141" s="8"/>
     </row>
     <row r="142" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG142" s="6"/>
-      <c r="AH142" s="108"/>
+      <c r="AH142" s="132"/>
       <c r="AI142" s="8"/>
     </row>
     <row r="143" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG143" s="6"/>
-      <c r="AH143" s="108"/>
+      <c r="AH143" s="132"/>
       <c r="AI143" s="8"/>
     </row>
     <row r="144" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG144" s="6"/>
-      <c r="AH144" s="108"/>
+      <c r="AH144" s="132"/>
       <c r="AI144" s="8"/>
     </row>
     <row r="145" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG145" s="6"/>
-      <c r="AH145" s="108"/>
+      <c r="AH145" s="132"/>
       <c r="AI145" s="8"/>
     </row>
     <row r="146" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG146" s="6"/>
-      <c r="AH146" s="108"/>
+      <c r="AH146" s="132"/>
       <c r="AI146" s="8"/>
     </row>
     <row r="147" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG147" s="6"/>
-      <c r="AH147" s="108"/>
+      <c r="AH147" s="132"/>
       <c r="AI147" s="8"/>
     </row>
     <row r="148" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG148" s="6"/>
-      <c r="AH148" s="108"/>
+      <c r="AH148" s="132"/>
       <c r="AI148" s="8"/>
     </row>
     <row r="149" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG149" s="6"/>
-      <c r="AH149" s="108"/>
+      <c r="AH149" s="132"/>
       <c r="AI149" s="8"/>
     </row>
     <row r="150" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG150" s="6"/>
-      <c r="AH150" s="108"/>
+      <c r="AH150" s="132"/>
       <c r="AI150" s="8"/>
     </row>
     <row r="151" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG151" s="6"/>
-      <c r="AH151" s="108"/>
+      <c r="AH151" s="132"/>
       <c r="AI151" s="8"/>
     </row>
     <row r="152" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG152" s="6"/>
-      <c r="AH152" s="108"/>
+      <c r="AH152" s="132"/>
       <c r="AI152" s="8"/>
     </row>
     <row r="153" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG153" s="6"/>
-      <c r="AH153" s="108"/>
+      <c r="AH153" s="132"/>
       <c r="AI153" s="8"/>
     </row>
     <row r="154" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG154" s="6"/>
-      <c r="AH154" s="108"/>
+      <c r="AH154" s="132"/>
       <c r="AI154" s="8"/>
     </row>
     <row r="155" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG155" s="6"/>
-      <c r="AH155" s="108"/>
+      <c r="AH155" s="132"/>
       <c r="AI155" s="8"/>
     </row>
     <row r="156" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG156" s="6"/>
-      <c r="AH156" s="108"/>
+      <c r="AH156" s="132"/>
       <c r="AI156" s="8"/>
     </row>
     <row r="157" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG157" s="6"/>
-      <c r="AH157" s="108"/>
+      <c r="AH157" s="132"/>
       <c r="AI157" s="8"/>
     </row>
     <row r="158" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG158" s="6"/>
-      <c r="AH158" s="108"/>
+      <c r="AH158" s="132"/>
       <c r="AI158" s="8"/>
     </row>
     <row r="159" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG159" s="6"/>
-      <c r="AH159" s="108"/>
+      <c r="AH159" s="132"/>
       <c r="AI159" s="8"/>
     </row>
     <row r="160" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG160" s="6"/>
-      <c r="AH160" s="108"/>
+      <c r="AH160" s="132"/>
       <c r="AI160" s="8"/>
     </row>
     <row r="161" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG161" s="6"/>
-      <c r="AH161" s="108"/>
+      <c r="AH161" s="132"/>
       <c r="AI161" s="8"/>
     </row>
     <row r="162" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG162" s="6"/>
-      <c r="AH162" s="108"/>
+      <c r="AH162" s="132"/>
       <c r="AI162" s="8"/>
     </row>
     <row r="163" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG163" s="6"/>
-      <c r="AH163" s="108"/>
+      <c r="AH163" s="132"/>
       <c r="AI163" s="8"/>
     </row>
     <row r="164" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG164" s="6"/>
-      <c r="AH164" s="108"/>
+      <c r="AH164" s="132"/>
       <c r="AI164" s="8"/>
     </row>
     <row r="165" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG165" s="6"/>
-      <c r="AH165" s="108"/>
+      <c r="AH165" s="132"/>
       <c r="AI165" s="8"/>
     </row>
     <row r="166" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG166" s="6"/>
-      <c r="AH166" s="108"/>
+      <c r="AH166" s="132"/>
       <c r="AI166" s="8"/>
     </row>
     <row r="167" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG167" s="6"/>
-      <c r="AH167" s="108"/>
+      <c r="AH167" s="132"/>
       <c r="AI167" s="8"/>
     </row>
     <row r="168" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG168" s="6"/>
-      <c r="AH168" s="108"/>
+      <c r="AH168" s="132"/>
       <c r="AI168" s="8"/>
     </row>
     <row r="169" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG169" s="6"/>
-      <c r="AH169" s="108"/>
+      <c r="AH169" s="132"/>
       <c r="AI169" s="8"/>
     </row>
     <row r="170" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG170" s="6"/>
-      <c r="AH170" s="108"/>
+      <c r="AH170" s="132"/>
       <c r="AI170" s="8"/>
     </row>
     <row r="171" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG171" s="6"/>
-      <c r="AH171" s="108"/>
+      <c r="AH171" s="132"/>
       <c r="AI171" s="8"/>
     </row>
     <row r="172" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG172" s="6"/>
-      <c r="AH172" s="108"/>
+      <c r="AH172" s="132"/>
       <c r="AI172" s="8"/>
     </row>
     <row r="173" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG173" s="6"/>
-      <c r="AH173" s="108"/>
+      <c r="AH173" s="132"/>
       <c r="AI173" s="8"/>
     </row>
     <row r="174" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG174" s="6"/>
-      <c r="AH174" s="108"/>
+      <c r="AH174" s="132"/>
       <c r="AI174" s="8"/>
     </row>
     <row r="175" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG175" s="6"/>
-      <c r="AH175" s="108"/>
+      <c r="AH175" s="132"/>
       <c r="AI175" s="8"/>
     </row>
     <row r="176" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG176" s="6"/>
-      <c r="AH176" s="108"/>
+      <c r="AH176" s="132"/>
       <c r="AI176" s="8"/>
     </row>
     <row r="177" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG177" s="6"/>
-      <c r="AH177" s="108"/>
+      <c r="AH177" s="132"/>
       <c r="AI177" s="8"/>
     </row>
     <row r="178" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG178" s="6"/>
-      <c r="AH178" s="108"/>
+      <c r="AH178" s="132"/>
       <c r="AI178" s="8"/>
     </row>
     <row r="179" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG179" s="6"/>
-      <c r="AH179" s="108"/>
+      <c r="AH179" s="132"/>
       <c r="AI179" s="8"/>
     </row>
     <row r="180" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG180" s="6"/>
-      <c r="AH180" s="108"/>
+      <c r="AH180" s="132"/>
       <c r="AI180" s="8"/>
     </row>
     <row r="181" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG181" s="6"/>
-      <c r="AH181" s="108"/>
+      <c r="AH181" s="132"/>
       <c r="AI181" s="8"/>
     </row>
     <row r="182" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG182" s="6"/>
-      <c r="AH182" s="108"/>
+      <c r="AH182" s="132"/>
       <c r="AI182" s="8"/>
     </row>
     <row r="183" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG183" s="6"/>
-      <c r="AH183" s="108"/>
+      <c r="AH183" s="132"/>
       <c r="AI183" s="8"/>
     </row>
     <row r="184" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG184" s="6"/>
-      <c r="AH184" s="108"/>
+      <c r="AH184" s="132"/>
       <c r="AI184" s="8"/>
     </row>
     <row r="185" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG185" s="6"/>
-      <c r="AH185" s="108"/>
+      <c r="AH185" s="132"/>
       <c r="AI185" s="8"/>
     </row>
     <row r="186" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG186" s="6"/>
-      <c r="AH186" s="108"/>
+      <c r="AH186" s="132"/>
       <c r="AI186" s="8"/>
     </row>
     <row r="187" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG187" s="6"/>
-      <c r="AH187" s="108"/>
+      <c r="AH187" s="132"/>
       <c r="AI187" s="8"/>
     </row>
     <row r="188" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG188" s="6"/>
-      <c r="AH188" s="108"/>
+      <c r="AH188" s="132"/>
       <c r="AI188" s="8"/>
     </row>
     <row r="189" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG189" s="6"/>
-      <c r="AH189" s="108"/>
+      <c r="AH189" s="132"/>
       <c r="AI189" s="8"/>
     </row>
     <row r="190" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG190" s="6"/>
-      <c r="AH190" s="108"/>
+      <c r="AH190" s="132"/>
       <c r="AI190" s="8"/>
     </row>
     <row r="191" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG191" s="6"/>
-      <c r="AH191" s="108"/>
+      <c r="AH191" s="132"/>
       <c r="AI191" s="8"/>
     </row>
     <row r="192" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG192" s="6"/>
-      <c r="AH192" s="108"/>
+      <c r="AH192" s="132"/>
       <c r="AI192" s="8"/>
     </row>
     <row r="193" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG193" s="6"/>
-      <c r="AH193" s="108"/>
+      <c r="AH193" s="132"/>
       <c r="AI193" s="8"/>
     </row>
     <row r="194" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG194" s="6"/>
-      <c r="AH194" s="108"/>
+      <c r="AH194" s="132"/>
       <c r="AI194" s="8"/>
     </row>
     <row r="195" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG195" s="6"/>
-      <c r="AH195" s="108"/>
+      <c r="AH195" s="132"/>
       <c r="AI195" s="8"/>
     </row>
     <row r="196" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG196" s="6"/>
-      <c r="AH196" s="108"/>
+      <c r="AH196" s="132"/>
       <c r="AI196" s="8"/>
     </row>
     <row r="197" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG197" s="6"/>
-      <c r="AH197" s="108"/>
+      <c r="AH197" s="132"/>
       <c r="AI197" s="8"/>
     </row>
     <row r="198" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG198" s="6"/>
-      <c r="AH198" s="108"/>
+      <c r="AH198" s="132"/>
       <c r="AI198" s="8"/>
     </row>
     <row r="199" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG199" s="6"/>
-      <c r="AH199" s="108"/>
+      <c r="AH199" s="132"/>
       <c r="AI199" s="8"/>
     </row>
     <row r="200" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG200" s="6"/>
-      <c r="AH200" s="108"/>
+      <c r="AH200" s="132"/>
       <c r="AI200" s="8"/>
     </row>
     <row r="201" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG201" s="6"/>
-      <c r="AH201" s="108"/>
+      <c r="AH201" s="132"/>
       <c r="AI201" s="8"/>
     </row>
     <row r="202" spans="33:35" x14ac:dyDescent="0.3">
       <c r="AG202" s="6"/>
-      <c r="AH202" s="108"/>
+      <c r="AH202" s="132"/>
       <c r="AI202" s="8"/>
     </row>
     <row r="203" spans="33:35" x14ac:dyDescent="0.3">
@@ -5453,9 +5409,9 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="AG6:AI6"/>
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="X6:AE6"/>
-    <mergeCell ref="AG6:AI6"/>
     <mergeCell ref="B1:E3"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="B6:E6"/>
@@ -5491,7 +5447,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="15" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -5562,63 +5518,63 @@
       <c r="R2" s="134"/>
       <c r="S2" s="134"/>
       <c r="T2" s="134"/>
-      <c r="X2" s="148" t="s">
+      <c r="X2" s="146" t="s">
         <v>33</v>
       </c>
-      <c r="Y2" s="148"/>
-      <c r="Z2" s="148"/>
-      <c r="AA2" s="148"/>
-      <c r="AB2" s="148"/>
-      <c r="AC2" s="148"/>
-      <c r="AD2" s="148"/>
-      <c r="AE2" s="148"/>
-      <c r="AF2" s="155" cm="1">
+      <c r="Y2" s="146"/>
+      <c r="Z2" s="146"/>
+      <c r="AA2" s="146"/>
+      <c r="AB2" s="146"/>
+      <c r="AC2" s="146"/>
+      <c r="AD2" s="146"/>
+      <c r="AE2" s="146"/>
+      <c r="AF2" s="143" cm="1">
         <f t="array" ref="AF2">project_start</f>
         <v>44330</v>
       </c>
-      <c r="AG2" s="155"/>
-      <c r="AH2" s="155"/>
-      <c r="AI2" s="155"/>
+      <c r="AG2" s="143"/>
+      <c r="AH2" s="143"/>
+      <c r="AI2" s="143"/>
       <c r="AJ2" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="AK2" s="155" cm="1">
+      <c r="AK2" s="143" cm="1">
         <f t="array" ref="AK2">project_end</f>
         <v>44531</v>
       </c>
-      <c r="AL2" s="155"/>
-      <c r="AM2" s="155"/>
-      <c r="AN2" s="155"/>
-      <c r="AO2" s="156" t="str" cm="1">
+      <c r="AL2" s="143"/>
+      <c r="AM2" s="143"/>
+      <c r="AN2" s="143"/>
+      <c r="AO2" s="144" t="str" cm="1">
         <f t="array" ref="AO2">"(" &amp; project_duration &amp; ")"</f>
         <v>(202)</v>
       </c>
-      <c r="AP2" s="156"/>
-      <c r="AT2" s="148" t="s">
+      <c r="AP2" s="144"/>
+      <c r="AT2" s="146" t="s">
         <v>28</v>
       </c>
-      <c r="AU2" s="148"/>
-      <c r="AV2" s="148"/>
-      <c r="AW2" s="148"/>
-      <c r="AX2" s="148"/>
-      <c r="AY2" s="148"/>
-      <c r="AZ2" s="148"/>
-      <c r="BA2" s="149" t="str">
+      <c r="AU2" s="146"/>
+      <c r="AV2" s="146"/>
+      <c r="AW2" s="146"/>
+      <c r="AX2" s="146"/>
+      <c r="AY2" s="146"/>
+      <c r="AZ2" s="146"/>
+      <c r="BA2" s="147" t="str">
         <f>Settings!D10</f>
         <v>F.Edward</v>
       </c>
-      <c r="BB2" s="149"/>
-      <c r="BC2" s="149"/>
-      <c r="BD2" s="149"/>
-      <c r="BE2" s="149"/>
-      <c r="BF2" s="149"/>
+      <c r="BB2" s="147"/>
+      <c r="BC2" s="147"/>
+      <c r="BD2" s="147"/>
+      <c r="BE2" s="147"/>
+      <c r="BF2" s="147"/>
       <c r="BL2" s="135" t="s">
         <v>25</v>
       </c>
-      <c r="BM2" s="154"/>
-      <c r="BN2" s="154"/>
-      <c r="BO2" s="154"/>
-      <c r="BP2" s="154"/>
+      <c r="BM2" s="142"/>
+      <c r="BN2" s="142"/>
+      <c r="BO2" s="142"/>
+      <c r="BP2" s="142"/>
       <c r="BQ2" s="136"/>
     </row>
     <row r="3" spans="1:69" s="4" customFormat="1" ht="6.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5648,76 +5604,76 @@
       <c r="D5" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="X5" s="150" t="s">
+      <c r="X5" s="138" t="s">
         <v>86</v>
       </c>
-      <c r="Y5" s="151"/>
-      <c r="Z5" s="151"/>
-      <c r="AA5" s="151"/>
-      <c r="AB5" s="151"/>
-      <c r="AC5" s="152"/>
-      <c r="AG5" s="150" t="s">
+      <c r="Y5" s="139"/>
+      <c r="Z5" s="139"/>
+      <c r="AA5" s="139"/>
+      <c r="AB5" s="139"/>
+      <c r="AC5" s="140"/>
+      <c r="AG5" s="138" t="s">
         <v>88</v>
       </c>
-      <c r="AH5" s="151"/>
-      <c r="AI5" s="151"/>
-      <c r="AJ5" s="151"/>
-      <c r="AK5" s="151"/>
-      <c r="AL5" s="152"/>
-      <c r="AP5" s="150" t="s">
+      <c r="AH5" s="139"/>
+      <c r="AI5" s="139"/>
+      <c r="AJ5" s="139"/>
+      <c r="AK5" s="139"/>
+      <c r="AL5" s="140"/>
+      <c r="AP5" s="138" t="s">
         <v>89</v>
       </c>
-      <c r="AQ5" s="151"/>
-      <c r="AR5" s="151"/>
-      <c r="AS5" s="151"/>
-      <c r="AT5" s="151"/>
-      <c r="AU5" s="152"/>
-      <c r="BL5" s="150" t="s">
+      <c r="AQ5" s="139"/>
+      <c r="AR5" s="139"/>
+      <c r="AS5" s="139"/>
+      <c r="AT5" s="139"/>
+      <c r="AU5" s="140"/>
+      <c r="BL5" s="138" t="s">
         <v>92</v>
       </c>
-      <c r="BM5" s="151"/>
-      <c r="BN5" s="151"/>
-      <c r="BO5" s="151"/>
-      <c r="BP5" s="151"/>
-      <c r="BQ5" s="152"/>
+      <c r="BM5" s="139"/>
+      <c r="BN5" s="139"/>
+      <c r="BO5" s="139"/>
+      <c r="BP5" s="139"/>
+      <c r="BQ5" s="140"/>
     </row>
     <row r="6" spans="1:69" x14ac:dyDescent="0.3">
       <c r="C6" s="16"/>
       <c r="D6" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="X6" s="153" t="s">
-        <v>133</v>
-      </c>
-      <c r="Y6" s="153"/>
-      <c r="Z6" s="153"/>
-      <c r="AA6" s="153"/>
-      <c r="AB6" s="153"/>
-      <c r="AC6" s="153"/>
-      <c r="AG6" s="153" t="s">
+      <c r="X6" s="141" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y6" s="141"/>
+      <c r="Z6" s="141"/>
+      <c r="AA6" s="141"/>
+      <c r="AB6" s="141"/>
+      <c r="AC6" s="141"/>
+      <c r="AG6" s="141" t="s">
         <v>94</v>
       </c>
-      <c r="AH6" s="153"/>
-      <c r="AI6" s="153"/>
-      <c r="AJ6" s="153"/>
-      <c r="AK6" s="153"/>
-      <c r="AL6" s="153"/>
-      <c r="AP6" s="153" t="s">
+      <c r="AH6" s="141"/>
+      <c r="AI6" s="141"/>
+      <c r="AJ6" s="141"/>
+      <c r="AK6" s="141"/>
+      <c r="AL6" s="141"/>
+      <c r="AP6" s="141" t="s">
         <v>90</v>
       </c>
-      <c r="AQ6" s="153"/>
-      <c r="AR6" s="153"/>
-      <c r="AS6" s="153"/>
-      <c r="AT6" s="153"/>
-      <c r="AU6" s="153"/>
-      <c r="BL6" s="157">
+      <c r="AQ6" s="141"/>
+      <c r="AR6" s="141"/>
+      <c r="AS6" s="141"/>
+      <c r="AT6" s="141"/>
+      <c r="AU6" s="141"/>
+      <c r="BL6" s="145">
         <v>44490</v>
       </c>
-      <c r="BM6" s="157"/>
-      <c r="BN6" s="157"/>
-      <c r="BO6" s="157"/>
-      <c r="BP6" s="157"/>
-      <c r="BQ6" s="157"/>
+      <c r="BM6" s="145"/>
+      <c r="BN6" s="145"/>
+      <c r="BO6" s="145"/>
+      <c r="BP6" s="145"/>
+      <c r="BQ6" s="145"/>
     </row>
     <row r="7" spans="1:69" x14ac:dyDescent="0.3">
       <c r="C7" s="17"/>
@@ -5925,353 +5881,353 @@
       <c r="C11" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="K11" s="139" t="s">
+      <c r="K11" s="152" t="s">
         <v>2</v>
       </c>
-      <c r="L11" s="139"/>
-      <c r="M11" s="139"/>
-      <c r="N11" s="139"/>
-      <c r="O11" s="139"/>
-      <c r="P11" s="139"/>
-      <c r="Q11" s="139"/>
-      <c r="R11" s="139"/>
-      <c r="S11" s="139"/>
-      <c r="T11" s="139"/>
-      <c r="U11" s="140" t="s">
+      <c r="L11" s="152"/>
+      <c r="M11" s="152"/>
+      <c r="N11" s="152"/>
+      <c r="O11" s="152"/>
+      <c r="P11" s="152"/>
+      <c r="Q11" s="152"/>
+      <c r="R11" s="152"/>
+      <c r="S11" s="152"/>
+      <c r="T11" s="152"/>
+      <c r="U11" s="153" t="s">
         <v>3</v>
       </c>
-      <c r="V11" s="140"/>
+      <c r="V11" s="153"/>
       <c r="W11" s="85" t="s">
         <v>93</v>
       </c>
-      <c r="X11" s="145" cm="1">
+      <c r="X11" s="148" cm="1">
         <f t="array" aca="1" ref="X11" ca="1">timeline_start+scroll_increment</f>
         <v>44343</v>
       </c>
-      <c r="Y11" s="145">
+      <c r="Y11" s="148">
         <f ca="1">X11+1</f>
         <v>44344</v>
       </c>
-      <c r="Z11" s="145">
+      <c r="Z11" s="148">
         <f t="shared" ref="Z11:BQ11" ca="1" si="1">Y11+1</f>
         <v>44345</v>
       </c>
-      <c r="AA11" s="145">
+      <c r="AA11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44346</v>
       </c>
-      <c r="AB11" s="145">
+      <c r="AB11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44347</v>
       </c>
-      <c r="AC11" s="145">
+      <c r="AC11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44348</v>
       </c>
-      <c r="AD11" s="145">
+      <c r="AD11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44349</v>
       </c>
-      <c r="AE11" s="145">
+      <c r="AE11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44350</v>
       </c>
-      <c r="AF11" s="145">
+      <c r="AF11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44351</v>
       </c>
-      <c r="AG11" s="145">
+      <c r="AG11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44352</v>
       </c>
-      <c r="AH11" s="145">
+      <c r="AH11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44353</v>
       </c>
-      <c r="AI11" s="145">
+      <c r="AI11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44354</v>
       </c>
-      <c r="AJ11" s="145">
+      <c r="AJ11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44355</v>
       </c>
-      <c r="AK11" s="145">
+      <c r="AK11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44356</v>
       </c>
-      <c r="AL11" s="145">
+      <c r="AL11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44357</v>
       </c>
-      <c r="AM11" s="145">
+      <c r="AM11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44358</v>
       </c>
-      <c r="AN11" s="145">
+      <c r="AN11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44359</v>
       </c>
-      <c r="AO11" s="145">
+      <c r="AO11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44360</v>
       </c>
-      <c r="AP11" s="145">
+      <c r="AP11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44361</v>
       </c>
-      <c r="AQ11" s="145">
+      <c r="AQ11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44362</v>
       </c>
-      <c r="AR11" s="145">
+      <c r="AR11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44363</v>
       </c>
-      <c r="AS11" s="145">
+      <c r="AS11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44364</v>
       </c>
-      <c r="AT11" s="145">
+      <c r="AT11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44365</v>
       </c>
-      <c r="AU11" s="145">
+      <c r="AU11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44366</v>
       </c>
-      <c r="AV11" s="145">
+      <c r="AV11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44367</v>
       </c>
-      <c r="AW11" s="145">
+      <c r="AW11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44368</v>
       </c>
-      <c r="AX11" s="145">
+      <c r="AX11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44369</v>
       </c>
-      <c r="AY11" s="145">
+      <c r="AY11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44370</v>
       </c>
-      <c r="AZ11" s="145">
+      <c r="AZ11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44371</v>
       </c>
-      <c r="BA11" s="145">
+      <c r="BA11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44372</v>
       </c>
-      <c r="BB11" s="145">
+      <c r="BB11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44373</v>
       </c>
-      <c r="BC11" s="145">
+      <c r="BC11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44374</v>
       </c>
-      <c r="BD11" s="145">
+      <c r="BD11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44375</v>
       </c>
-      <c r="BE11" s="145">
+      <c r="BE11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44376</v>
       </c>
-      <c r="BF11" s="145">
+      <c r="BF11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44377</v>
       </c>
-      <c r="BG11" s="145">
+      <c r="BG11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44378</v>
       </c>
-      <c r="BH11" s="145">
+      <c r="BH11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44379</v>
       </c>
-      <c r="BI11" s="145">
+      <c r="BI11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44380</v>
       </c>
-      <c r="BJ11" s="145">
+      <c r="BJ11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44381</v>
       </c>
-      <c r="BK11" s="145">
+      <c r="BK11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44382</v>
       </c>
-      <c r="BL11" s="145">
+      <c r="BL11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44383</v>
       </c>
-      <c r="BM11" s="145">
+      <c r="BM11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44384</v>
       </c>
-      <c r="BN11" s="145">
+      <c r="BN11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44385</v>
       </c>
-      <c r="BO11" s="145">
+      <c r="BO11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44386</v>
       </c>
-      <c r="BP11" s="145">
+      <c r="BP11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44387</v>
       </c>
-      <c r="BQ11" s="145">
+      <c r="BQ11" s="148">
         <f t="shared" ca="1" si="1"/>
         <v>44388</v>
       </c>
     </row>
     <row r="12" spans="1:69" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K12" s="141" t="s">
+      <c r="K12" s="154" t="s">
         <v>4</v>
       </c>
-      <c r="L12" s="141"/>
-      <c r="M12" s="141"/>
-      <c r="N12" s="141"/>
-      <c r="O12" s="141"/>
-      <c r="P12" s="141"/>
-      <c r="Q12" s="141"/>
-      <c r="R12" s="141"/>
-      <c r="S12" s="141"/>
-      <c r="T12" s="141"/>
-      <c r="U12" s="142" t="s">
+      <c r="L12" s="154"/>
+      <c r="M12" s="154"/>
+      <c r="N12" s="154"/>
+      <c r="O12" s="154"/>
+      <c r="P12" s="154"/>
+      <c r="Q12" s="154"/>
+      <c r="R12" s="154"/>
+      <c r="S12" s="154"/>
+      <c r="T12" s="154"/>
+      <c r="U12" s="155" t="s">
         <v>5</v>
       </c>
-      <c r="V12" s="142"/>
+      <c r="V12" s="155"/>
       <c r="W12" s="85">
         <v>17</v>
       </c>
-      <c r="X12" s="145"/>
-      <c r="Y12" s="145"/>
-      <c r="Z12" s="145"/>
-      <c r="AA12" s="145"/>
-      <c r="AB12" s="145"/>
-      <c r="AC12" s="145"/>
-      <c r="AD12" s="145"/>
-      <c r="AE12" s="145"/>
-      <c r="AF12" s="145"/>
-      <c r="AG12" s="145"/>
-      <c r="AH12" s="145"/>
-      <c r="AI12" s="145"/>
-      <c r="AJ12" s="145"/>
-      <c r="AK12" s="145"/>
-      <c r="AL12" s="145"/>
-      <c r="AM12" s="145"/>
-      <c r="AN12" s="145"/>
-      <c r="AO12" s="145"/>
-      <c r="AP12" s="145"/>
-      <c r="AQ12" s="145"/>
-      <c r="AR12" s="145"/>
-      <c r="AS12" s="145"/>
-      <c r="AT12" s="145"/>
-      <c r="AU12" s="145"/>
-      <c r="AV12" s="145"/>
-      <c r="AW12" s="145"/>
-      <c r="AX12" s="145"/>
-      <c r="AY12" s="145"/>
-      <c r="AZ12" s="145"/>
-      <c r="BA12" s="145"/>
-      <c r="BB12" s="145"/>
-      <c r="BC12" s="145"/>
-      <c r="BD12" s="145"/>
-      <c r="BE12" s="145"/>
-      <c r="BF12" s="145"/>
-      <c r="BG12" s="145"/>
-      <c r="BH12" s="145"/>
-      <c r="BI12" s="145"/>
-      <c r="BJ12" s="145"/>
-      <c r="BK12" s="145"/>
-      <c r="BL12" s="145"/>
-      <c r="BM12" s="145"/>
-      <c r="BN12" s="145"/>
-      <c r="BO12" s="145"/>
-      <c r="BP12" s="145"/>
-      <c r="BQ12" s="145"/>
+      <c r="X12" s="148"/>
+      <c r="Y12" s="148"/>
+      <c r="Z12" s="148"/>
+      <c r="AA12" s="148"/>
+      <c r="AB12" s="148"/>
+      <c r="AC12" s="148"/>
+      <c r="AD12" s="148"/>
+      <c r="AE12" s="148"/>
+      <c r="AF12" s="148"/>
+      <c r="AG12" s="148"/>
+      <c r="AH12" s="148"/>
+      <c r="AI12" s="148"/>
+      <c r="AJ12" s="148"/>
+      <c r="AK12" s="148"/>
+      <c r="AL12" s="148"/>
+      <c r="AM12" s="148"/>
+      <c r="AN12" s="148"/>
+      <c r="AO12" s="148"/>
+      <c r="AP12" s="148"/>
+      <c r="AQ12" s="148"/>
+      <c r="AR12" s="148"/>
+      <c r="AS12" s="148"/>
+      <c r="AT12" s="148"/>
+      <c r="AU12" s="148"/>
+      <c r="AV12" s="148"/>
+      <c r="AW12" s="148"/>
+      <c r="AX12" s="148"/>
+      <c r="AY12" s="148"/>
+      <c r="AZ12" s="148"/>
+      <c r="BA12" s="148"/>
+      <c r="BB12" s="148"/>
+      <c r="BC12" s="148"/>
+      <c r="BD12" s="148"/>
+      <c r="BE12" s="148"/>
+      <c r="BF12" s="148"/>
+      <c r="BG12" s="148"/>
+      <c r="BH12" s="148"/>
+      <c r="BI12" s="148"/>
+      <c r="BJ12" s="148"/>
+      <c r="BK12" s="148"/>
+      <c r="BL12" s="148"/>
+      <c r="BM12" s="148"/>
+      <c r="BN12" s="148"/>
+      <c r="BO12" s="148"/>
+      <c r="BP12" s="148"/>
+      <c r="BQ12" s="148"/>
     </row>
     <row r="13" spans="1:69" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="138" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="138"/>
-      <c r="D13" s="138"/>
-      <c r="E13" s="138" t="s">
+      <c r="B13" s="151" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="151"/>
+      <c r="D13" s="151"/>
+      <c r="E13" s="151" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="138"/>
-      <c r="G13" s="138"/>
-      <c r="H13" s="138"/>
-      <c r="I13" s="138"/>
-      <c r="J13" s="138"/>
-      <c r="K13" s="144">
+      <c r="F13" s="151"/>
+      <c r="G13" s="151"/>
+      <c r="H13" s="151"/>
+      <c r="I13" s="151"/>
+      <c r="J13" s="151"/>
+      <c r="K13" s="157">
         <v>44319</v>
       </c>
-      <c r="L13" s="144"/>
-      <c r="M13" s="144"/>
-      <c r="N13" s="144"/>
-      <c r="O13" s="144"/>
-      <c r="P13" s="144"/>
-      <c r="Q13" s="144"/>
-      <c r="R13" s="144"/>
-      <c r="S13" s="144"/>
-      <c r="T13" s="144"/>
-      <c r="U13" s="143">
+      <c r="L13" s="157"/>
+      <c r="M13" s="157"/>
+      <c r="N13" s="157"/>
+      <c r="O13" s="157"/>
+      <c r="P13" s="157"/>
+      <c r="Q13" s="157"/>
+      <c r="R13" s="157"/>
+      <c r="S13" s="157"/>
+      <c r="T13" s="157"/>
+      <c r="U13" s="156">
         <v>44319</v>
       </c>
-      <c r="V13" s="143"/>
-      <c r="X13" s="145"/>
-      <c r="Y13" s="145"/>
-      <c r="Z13" s="145"/>
-      <c r="AA13" s="145"/>
-      <c r="AB13" s="145"/>
-      <c r="AC13" s="145"/>
-      <c r="AD13" s="145"/>
-      <c r="AE13" s="145"/>
-      <c r="AF13" s="145"/>
-      <c r="AG13" s="145"/>
-      <c r="AH13" s="145"/>
-      <c r="AI13" s="145"/>
-      <c r="AJ13" s="145"/>
-      <c r="AK13" s="145"/>
-      <c r="AL13" s="145"/>
-      <c r="AM13" s="145"/>
-      <c r="AN13" s="145"/>
-      <c r="AO13" s="145"/>
-      <c r="AP13" s="145"/>
-      <c r="AQ13" s="145"/>
-      <c r="AR13" s="145"/>
-      <c r="AS13" s="145"/>
-      <c r="AT13" s="145"/>
-      <c r="AU13" s="145"/>
-      <c r="AV13" s="145"/>
-      <c r="AW13" s="145"/>
-      <c r="AX13" s="145"/>
-      <c r="AY13" s="145"/>
-      <c r="AZ13" s="145"/>
-      <c r="BA13" s="145"/>
-      <c r="BB13" s="145"/>
-      <c r="BC13" s="145"/>
-      <c r="BD13" s="145"/>
-      <c r="BE13" s="145"/>
-      <c r="BF13" s="145"/>
-      <c r="BG13" s="145"/>
-      <c r="BH13" s="145"/>
-      <c r="BI13" s="145"/>
-      <c r="BJ13" s="145"/>
-      <c r="BK13" s="145"/>
-      <c r="BL13" s="145"/>
-      <c r="BM13" s="145"/>
-      <c r="BN13" s="145"/>
-      <c r="BO13" s="145"/>
-      <c r="BP13" s="145"/>
-      <c r="BQ13" s="145"/>
+      <c r="V13" s="156"/>
+      <c r="X13" s="148"/>
+      <c r="Y13" s="148"/>
+      <c r="Z13" s="148"/>
+      <c r="AA13" s="148"/>
+      <c r="AB13" s="148"/>
+      <c r="AC13" s="148"/>
+      <c r="AD13" s="148"/>
+      <c r="AE13" s="148"/>
+      <c r="AF13" s="148"/>
+      <c r="AG13" s="148"/>
+      <c r="AH13" s="148"/>
+      <c r="AI13" s="148"/>
+      <c r="AJ13" s="148"/>
+      <c r="AK13" s="148"/>
+      <c r="AL13" s="148"/>
+      <c r="AM13" s="148"/>
+      <c r="AN13" s="148"/>
+      <c r="AO13" s="148"/>
+      <c r="AP13" s="148"/>
+      <c r="AQ13" s="148"/>
+      <c r="AR13" s="148"/>
+      <c r="AS13" s="148"/>
+      <c r="AT13" s="148"/>
+      <c r="AU13" s="148"/>
+      <c r="AV13" s="148"/>
+      <c r="AW13" s="148"/>
+      <c r="AX13" s="148"/>
+      <c r="AY13" s="148"/>
+      <c r="AZ13" s="148"/>
+      <c r="BA13" s="148"/>
+      <c r="BB13" s="148"/>
+      <c r="BC13" s="148"/>
+      <c r="BD13" s="148"/>
+      <c r="BE13" s="148"/>
+      <c r="BF13" s="148"/>
+      <c r="BG13" s="148"/>
+      <c r="BH13" s="148"/>
+      <c r="BI13" s="148"/>
+      <c r="BJ13" s="148"/>
+      <c r="BK13" s="148"/>
+      <c r="BL13" s="148"/>
+      <c r="BM13" s="148"/>
+      <c r="BN13" s="148"/>
+      <c r="BO13" s="148"/>
+      <c r="BP13" s="148"/>
+      <c r="BQ13" s="148"/>
     </row>
     <row r="14" spans="1:69" s="36" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="76"/>
@@ -6309,10 +6265,10 @@
       <c r="M14" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="N14" s="146" t="s">
+      <c r="N14" s="149" t="s">
         <v>14</v>
       </c>
-      <c r="O14" s="147"/>
+      <c r="O14" s="150"/>
       <c r="P14" s="29" t="s">
         <v>15</v>
       </c>
@@ -13917,18 +13873,49 @@
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="X5:AC5"/>
-    <mergeCell ref="X6:AC6"/>
-    <mergeCell ref="BL2:BQ2"/>
-    <mergeCell ref="AF2:AI2"/>
-    <mergeCell ref="AK2:AN2"/>
-    <mergeCell ref="AG5:AL5"/>
-    <mergeCell ref="AG6:AL6"/>
-    <mergeCell ref="AP5:AU5"/>
-    <mergeCell ref="AP6:AU6"/>
-    <mergeCell ref="AO2:AP2"/>
-    <mergeCell ref="BL5:BQ5"/>
-    <mergeCell ref="BL6:BQ6"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:J13"/>
+    <mergeCell ref="K11:T11"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="K12:T12"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="K13:T13"/>
+    <mergeCell ref="AH11:AH13"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="X11:X13"/>
+    <mergeCell ref="Y11:Y13"/>
+    <mergeCell ref="Z11:Z13"/>
+    <mergeCell ref="AA11:AA13"/>
+    <mergeCell ref="AB11:AB13"/>
+    <mergeCell ref="AC11:AC13"/>
+    <mergeCell ref="AD11:AD13"/>
+    <mergeCell ref="AE11:AE13"/>
+    <mergeCell ref="AF11:AF13"/>
+    <mergeCell ref="AG11:AG13"/>
+    <mergeCell ref="AT11:AT13"/>
+    <mergeCell ref="AI11:AI13"/>
+    <mergeCell ref="AJ11:AJ13"/>
+    <mergeCell ref="AK11:AK13"/>
+    <mergeCell ref="AL11:AL13"/>
+    <mergeCell ref="AM11:AM13"/>
+    <mergeCell ref="AN11:AN13"/>
+    <mergeCell ref="AO11:AO13"/>
+    <mergeCell ref="AP11:AP13"/>
+    <mergeCell ref="AQ11:AQ13"/>
+    <mergeCell ref="AR11:AR13"/>
+    <mergeCell ref="AS11:AS13"/>
+    <mergeCell ref="BQ11:BQ13"/>
+    <mergeCell ref="AV11:AV13"/>
+    <mergeCell ref="AW11:AW13"/>
+    <mergeCell ref="AX11:AX13"/>
+    <mergeCell ref="AY11:AY13"/>
+    <mergeCell ref="AZ11:AZ13"/>
+    <mergeCell ref="BL11:BL13"/>
+    <mergeCell ref="BM11:BM13"/>
+    <mergeCell ref="BN11:BN13"/>
+    <mergeCell ref="BO11:BO13"/>
+    <mergeCell ref="BP11:BP13"/>
     <mergeCell ref="B1:T3"/>
     <mergeCell ref="AT2:AZ2"/>
     <mergeCell ref="BA2:BF2"/>
@@ -13945,49 +13932,18 @@
     <mergeCell ref="BE11:BE13"/>
     <mergeCell ref="BF11:BF13"/>
     <mergeCell ref="AU11:AU13"/>
-    <mergeCell ref="BQ11:BQ13"/>
-    <mergeCell ref="AV11:AV13"/>
-    <mergeCell ref="AW11:AW13"/>
-    <mergeCell ref="AX11:AX13"/>
-    <mergeCell ref="AY11:AY13"/>
-    <mergeCell ref="AZ11:AZ13"/>
-    <mergeCell ref="BL11:BL13"/>
-    <mergeCell ref="BM11:BM13"/>
-    <mergeCell ref="BN11:BN13"/>
-    <mergeCell ref="BO11:BO13"/>
-    <mergeCell ref="BP11:BP13"/>
-    <mergeCell ref="AT11:AT13"/>
-    <mergeCell ref="AI11:AI13"/>
-    <mergeCell ref="AJ11:AJ13"/>
-    <mergeCell ref="AK11:AK13"/>
-    <mergeCell ref="AL11:AL13"/>
-    <mergeCell ref="AM11:AM13"/>
-    <mergeCell ref="AN11:AN13"/>
-    <mergeCell ref="AO11:AO13"/>
-    <mergeCell ref="AP11:AP13"/>
-    <mergeCell ref="AQ11:AQ13"/>
-    <mergeCell ref="AR11:AR13"/>
-    <mergeCell ref="AS11:AS13"/>
-    <mergeCell ref="AH11:AH13"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="X11:X13"/>
-    <mergeCell ref="Y11:Y13"/>
-    <mergeCell ref="Z11:Z13"/>
-    <mergeCell ref="AA11:AA13"/>
-    <mergeCell ref="AB11:AB13"/>
-    <mergeCell ref="AC11:AC13"/>
-    <mergeCell ref="AD11:AD13"/>
-    <mergeCell ref="AE11:AE13"/>
-    <mergeCell ref="AF11:AF13"/>
-    <mergeCell ref="AG11:AG13"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:J13"/>
-    <mergeCell ref="K11:T11"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="K12:T12"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="K13:T13"/>
+    <mergeCell ref="X5:AC5"/>
+    <mergeCell ref="X6:AC6"/>
+    <mergeCell ref="BL2:BQ2"/>
+    <mergeCell ref="AF2:AI2"/>
+    <mergeCell ref="AK2:AN2"/>
+    <mergeCell ref="AG5:AL5"/>
+    <mergeCell ref="AG6:AL6"/>
+    <mergeCell ref="AP5:AU5"/>
+    <mergeCell ref="AP6:AU6"/>
+    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="BL5:BQ5"/>
+    <mergeCell ref="BL6:BQ6"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <conditionalFormatting sqref="X11:BQ49">
@@ -14006,92 +13962,92 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16:G49">
-    <cfRule type="expression" dxfId="94" priority="161" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="12" stopIfTrue="1">
+      <formula>OR(colour_code=9901,colour_code=9902)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="93" priority="133" stopIfTrue="1">
+      <formula>OR(colour_code=101,colour_code=104)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="92" priority="134" stopIfTrue="1">
+      <formula>OR(colour_code=102,colour_code=103)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="91" priority="135" stopIfTrue="1">
+      <formula>OR(colour_code=201,colour_code=204)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="90" priority="136" stopIfTrue="1">
+      <formula>OR(colour_code=202,colour_code=203)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="89" priority="137" stopIfTrue="1">
+      <formula>OR(colour_code=301,colour_code=304)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="138" stopIfTrue="1">
+      <formula>OR(colour_code=302,colour_code=303)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="87" priority="139" stopIfTrue="1">
+      <formula>OR(colour_code=401,colour_code=404)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="86" priority="140" stopIfTrue="1">
+      <formula>OR(colour_code=402,colour_code=403)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="85" priority="141" stopIfTrue="1">
+      <formula>OR(colour_code=501,colour_code=504)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="84" priority="142" stopIfTrue="1">
+      <formula>OR(colour_code=502,colour_code=503)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="83" priority="143" stopIfTrue="1">
+      <formula>OR(colour_code=601,colour_code=604)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="82" priority="144" stopIfTrue="1">
+      <formula>OR(colour_code=602,colour_code=603)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="81" priority="145" stopIfTrue="1">
+      <formula>OR(colour_code=701,colour_code=704)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="80" priority="147" stopIfTrue="1">
+      <formula>OR(colour_code=702,colour_code=703)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="79" priority="148" stopIfTrue="1">
+      <formula>OR(colour_code=801,colour_code=804)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="78" priority="149" stopIfTrue="1">
+      <formula>OR(colour_code=802,colour_code=803)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="77" priority="150" stopIfTrue="1">
+      <formula>OR(colour_code=901,colour_code=904)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="76" priority="151" stopIfTrue="1">
+      <formula>OR(colour_code=902,colour_code=903)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="75" priority="152" stopIfTrue="1">
+      <formula>OR(colour_code=1001,colour_code=1004)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="74" priority="153" stopIfTrue="1">
+      <formula>OR(colour_code=1002,colour_code=1003)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="73" priority="154" stopIfTrue="1">
+      <formula>OR(colour_code=1101,colour_code=1104)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="72" priority="155" stopIfTrue="1">
+      <formula>OR(colour_code=1102,colour_code=1103)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="71" priority="156" stopIfTrue="1">
+      <formula>OR(colour_code=1201,colour_code=1204)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="158" stopIfTrue="1">
+      <formula>OR(colour_code=1202,colour_code=1203)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="69" priority="159" stopIfTrue="1">
+      <formula>OR(colour_code=1301,colour_code=1304)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="160" stopIfTrue="1">
+      <formula>OR(colour_code=1302,colour_code=1303)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="161" stopIfTrue="1">
       <formula>OR(colour_code=1401,colour_code=1404)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="163" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="163" stopIfTrue="1">
       <formula>OR(colour_code=1402,colour_code=1403)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="92" priority="159" stopIfTrue="1">
-      <formula>OR(colour_code=1301,colour_code=1304)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="91" priority="160" stopIfTrue="1">
-      <formula>OR(colour_code=1302,colour_code=1303)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="90" priority="156" stopIfTrue="1">
-      <formula>OR(colour_code=1201,colour_code=1204)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="89" priority="158" stopIfTrue="1">
-      <formula>OR(colour_code=1202,colour_code=1203)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="88" priority="154" stopIfTrue="1">
-      <formula>OR(colour_code=1101,colour_code=1104)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="87" priority="155" stopIfTrue="1">
-      <formula>OR(colour_code=1102,colour_code=1103)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="86" priority="152" stopIfTrue="1">
-      <formula>OR(colour_code=1001,colour_code=1004)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="85" priority="153" stopIfTrue="1">
-      <formula>OR(colour_code=1002,colour_code=1003)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="84" priority="150" stopIfTrue="1">
-      <formula>OR(colour_code=901,colour_code=904)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="83" priority="151" stopIfTrue="1">
-      <formula>OR(colour_code=902,colour_code=903)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="82" priority="12" stopIfTrue="1">
-      <formula>OR(colour_code=9901,colour_code=9902)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="81" priority="133" stopIfTrue="1">
-      <formula>OR(colour_code=101,colour_code=104)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="80" priority="134" stopIfTrue="1">
-      <formula>OR(colour_code=102,colour_code=103)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="79" priority="135" stopIfTrue="1">
-      <formula>OR(colour_code=201,colour_code=204)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="78" priority="136" stopIfTrue="1">
-      <formula>OR(colour_code=202,colour_code=203)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="77" priority="137" stopIfTrue="1">
-      <formula>OR(colour_code=301,colour_code=304)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="76" priority="138" stopIfTrue="1">
-      <formula>OR(colour_code=302,colour_code=303)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="75" priority="139" stopIfTrue="1">
-      <formula>OR(colour_code=401,colour_code=404)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="74" priority="140" stopIfTrue="1">
-      <formula>OR(colour_code=402,colour_code=403)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="73" priority="141" stopIfTrue="1">
-      <formula>OR(colour_code=501,colour_code=504)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="72" priority="142" stopIfTrue="1">
-      <formula>OR(colour_code=502,colour_code=503)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="71" priority="143" stopIfTrue="1">
-      <formula>OR(colour_code=601,colour_code=604)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="70" priority="144" stopIfTrue="1">
-      <formula>OR(colour_code=602,colour_code=603)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="69" priority="145" stopIfTrue="1">
-      <formula>OR(colour_code=701,colour_code=704)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="68" priority="147" stopIfTrue="1">
-      <formula>OR(colour_code=702,colour_code=703)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="148" stopIfTrue="1">
-      <formula>OR(colour_code=801,colour_code=804)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="66" priority="149" stopIfTrue="1">
-      <formula>OR(colour_code=802,colour_code=803)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="65" priority="171" stopIfTrue="1">
       <formula>OR(colour_code=802,colour_code=803)</formula>
@@ -14197,68 +14153,68 @@
     <cfRule type="expression" dxfId="33" priority="108" stopIfTrue="1">
       <formula>OR(colour_code=803,colour_code=804)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="174" stopIfTrue="1">
-      <formula>colour_code=1</formula>
+    <cfRule type="expression" dxfId="32" priority="109" stopIfTrue="1">
+      <formula>colour_code=901</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="180" stopIfTrue="1">
-      <formula>colour_code=2</formula>
+    <cfRule type="expression" dxfId="31" priority="110" stopIfTrue="1">
+      <formula>colour_code=902</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="181" stopIfTrue="1">
-      <formula>colour_code=3</formula>
+    <cfRule type="expression" dxfId="30" priority="111" stopIfTrue="1">
+      <formula>OR(colour_code=903,colour_code=904)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="132" stopIfTrue="1">
-      <formula>OR(colour_code=1403,colour_code=1404)</formula>
+    <cfRule type="expression" dxfId="29" priority="112" stopIfTrue="1">
+      <formula>colour_code=1001</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="131" stopIfTrue="1">
-      <formula>colour_code=1402</formula>
+    <cfRule type="expression" dxfId="28" priority="113" stopIfTrue="1">
+      <formula>colour_code=1002</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="130" stopIfTrue="1">
-      <formula>colour_code=1401</formula>
+    <cfRule type="expression" dxfId="27" priority="114" stopIfTrue="1">
+      <formula>OR(colour_code=1003,colour_code=1004)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="127" stopIfTrue="1">
-      <formula>colour_code=1301</formula>
+    <cfRule type="expression" dxfId="26" priority="115" stopIfTrue="1">
+      <formula>colour_code=1101</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="128" stopIfTrue="1">
-      <formula>colour_code=1302</formula>
+    <cfRule type="expression" dxfId="25" priority="116" stopIfTrue="1">
+      <formula>colour_code=1102</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="129" stopIfTrue="1">
-      <formula>OR(colour_code=1303,colour_code=1304)</formula>
+    <cfRule type="expression" dxfId="24" priority="117" stopIfTrue="1">
+      <formula>OR(colour_code=1103,colour_code=1104)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="126" stopIfTrue="1">
-      <formula>OR(colour_code=1203,colour_code=1204)</formula>
+    <cfRule type="expression" dxfId="23" priority="118" stopIfTrue="1">
+      <formula>colour_code=1201</formula>
     </cfRule>
     <cfRule type="expression" dxfId="22" priority="125" stopIfTrue="1">
       <formula>colour_code=1202</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="118" stopIfTrue="1">
-      <formula>colour_code=1201</formula>
+    <cfRule type="expression" dxfId="21" priority="126" stopIfTrue="1">
+      <formula>OR(colour_code=1203,colour_code=1204)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="117" stopIfTrue="1">
-      <formula>OR(colour_code=1103,colour_code=1104)</formula>
+    <cfRule type="expression" dxfId="20" priority="127" stopIfTrue="1">
+      <formula>colour_code=1301</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="116" stopIfTrue="1">
-      <formula>colour_code=1102</formula>
+    <cfRule type="expression" dxfId="19" priority="128" stopIfTrue="1">
+      <formula>colour_code=1302</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="115" stopIfTrue="1">
-      <formula>colour_code=1101</formula>
+    <cfRule type="expression" dxfId="18" priority="129" stopIfTrue="1">
+      <formula>OR(colour_code=1303,colour_code=1304)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="114" stopIfTrue="1">
-      <formula>OR(colour_code=1003,colour_code=1004)</formula>
+    <cfRule type="expression" dxfId="17" priority="130" stopIfTrue="1">
+      <formula>colour_code=1401</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="113" stopIfTrue="1">
-      <formula>colour_code=1002</formula>
+    <cfRule type="expression" dxfId="16" priority="131" stopIfTrue="1">
+      <formula>colour_code=1402</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="112" stopIfTrue="1">
-      <formula>colour_code=1001</formula>
+    <cfRule type="expression" dxfId="15" priority="132" stopIfTrue="1">
+      <formula>OR(colour_code=1403,colour_code=1404)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="111" stopIfTrue="1">
-      <formula>OR(colour_code=903,colour_code=904)</formula>
+    <cfRule type="expression" dxfId="14" priority="174" stopIfTrue="1">
+      <formula>colour_code=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="110" stopIfTrue="1">
-      <formula>colour_code=902</formula>
+    <cfRule type="expression" dxfId="13" priority="180" stopIfTrue="1">
+      <formula>colour_code=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="109" stopIfTrue="1">
-      <formula>colour_code=901</formula>
+    <cfRule type="expression" dxfId="12" priority="181" stopIfTrue="1">
+      <formula>colour_code=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16:L49">
@@ -14419,12 +14375,54 @@
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{398EECAF-DB5B-4A0B-8CE8-8C260DF5E49C}">
           <x14:formula1>
             <xm:f>OFFSET(Settings!$N$9,,,COUNTA(Settings!$N$9:$N$35))</xm:f>
           </x14:formula1>
           <xm:sqref>I16:I49</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{40153C05-7F87-4744-BC7D-22E66EC20E45}">
+          <x14:formula1>
+            <xm:f>OFFSET(Settings!$AH$9,,,COUNTA(Settings!$AH$9:$AH204))</xm:f>
+          </x14:formula1>
+          <xm:sqref>F16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{46F226F2-A2D8-484C-892B-229EB560A264}">
+          <x14:formula1>
+            <xm:f>OFFSET(Settings!$AH$9,,,COUNTA(Settings!$AH$9:$AH204))</xm:f>
+          </x14:formula1>
+          <xm:sqref>F21</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{447ED948-A5BC-4D5E-8223-F1849C47BD91}">
+          <x14:formula1>
+            <xm:f>OFFSET(Settings!$AH$9,,,COUNTA(Settings!$AH$9:$AH204))</xm:f>
+          </x14:formula1>
+          <xm:sqref>F26</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B3EE530F-6D9A-49A2-A0C5-022D214CD4CC}">
+          <x14:formula1>
+            <xm:f>OFFSET(Settings!$AH$9,,,COUNTA(Settings!$AH$9:$AH204))</xm:f>
+          </x14:formula1>
+          <xm:sqref>F31</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{61ACB373-9A02-496D-B137-A0139CA8FFDE}">
+          <x14:formula1>
+            <xm:f>OFFSET(Settings!$AH$9,,,COUNTA(Settings!$AH$9:$AH204))</xm:f>
+          </x14:formula1>
+          <xm:sqref>F36</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{628CB2B5-86F5-4FC4-943E-9916DCD6B6EF}">
+          <x14:formula1>
+            <xm:f>OFFSET(Settings!$AH$9,,,COUNTA(Settings!$AH$9:$AH204))</xm:f>
+          </x14:formula1>
+          <xm:sqref>F42</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EBD7DD96-7C94-4BA5-B31F-85AFD7DA4426}">
+          <x14:formula1>
+            <xm:f>OFFSET(Settings!$AH$9,,,COUNTA(Settings!$AH$9:$AH204))</xm:f>
+          </x14:formula1>
+          <xm:sqref>F46</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -14490,69 +14488,69 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="29.4" x14ac:dyDescent="0.65"/>
   <cols>
-    <col min="1" max="1" width="2.3984375" style="126" customWidth="1"/>
-    <col min="2" max="16384" width="8.796875" style="126"/>
+    <col min="1" max="1" width="2.3984375" style="123" customWidth="1"/>
+    <col min="2" max="16384" width="8.796875" style="123"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2" x14ac:dyDescent="0.65">
-      <c r="B1" s="130" t="s">
-        <v>134</v>
+      <c r="B1" s="127" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.65">
-      <c r="B2" s="130"/>
+      <c r="B2" s="127"/>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.65">
-      <c r="B3" s="131" t="s">
-        <v>143</v>
+      <c r="B3" s="128" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.65">
-      <c r="B4" s="132" t="s">
-        <v>144</v>
+      <c r="B4" s="129" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="400" spans="2:2" x14ac:dyDescent="0.65">
-      <c r="B400" s="126" t="s">
-        <v>131</v>
+      <c r="B400" s="123" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="401" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B401" s="126" t="s">
-        <v>135</v>
+      <c r="B401" s="123" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="402" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B402" s="127" t="s">
-        <v>136</v>
+      <c r="B402" s="124" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="403" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B403" s="127" t="s">
-        <v>137</v>
+      <c r="B403" s="124" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="405" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B405" s="126" t="s">
-        <v>132</v>
+      <c r="B405" s="123" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="406" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B406" s="126" t="s">
-        <v>138</v>
+      <c r="B406" s="123" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="407" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B407" s="126" t="s">
-        <v>139</v>
-      </c>
-      <c r="D407" s="128" t="s">
-        <v>140</v>
+      <c r="B407" s="123" t="s">
+        <v>128</v>
+      </c>
+      <c r="D407" s="125" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="409" spans="2:4" x14ac:dyDescent="0.65">
-      <c r="B409" s="126" t="s">
-        <v>141</v>
+      <c r="B409" s="123" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>